<commit_message>
[DHTD-53] presentation and data added
</commit_message>
<xml_diff>
--- a/midterm-presentation/TimeSheet.xlsx
+++ b/midterm-presentation/TimeSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TowerDefense\midterm-presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC70C26-7FF4-4C7A-A631-C0707BFC4180}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26970FA-1DAA-42C2-9CCF-84410A299BC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="115">
   <si>
     <t>Ticketart</t>
   </si>
@@ -304,9 +304,6 @@
     <t>Overall Time Spent (h)</t>
   </si>
   <si>
-    <t>build towers</t>
-  </si>
-  <si>
     <t>return to main menu</t>
   </si>
   <si>
@@ -323,6 +320,63 @@
   </si>
   <si>
     <t>Testing (h)</t>
+  </si>
+  <si>
+    <t>DHTD-38</t>
+  </si>
+  <si>
+    <t>GE: Build towers when a button is clicked</t>
+  </si>
+  <si>
+    <t>build towers on selected area</t>
+  </si>
+  <si>
+    <t>DHTD-49</t>
+  </si>
+  <si>
+    <t>GE: remove Tower on click</t>
+  </si>
+  <si>
+    <t>DHTD-50</t>
+  </si>
+  <si>
+    <t>GE: spawn wave button</t>
+  </si>
+  <si>
+    <t>DHTD-46</t>
+  </si>
+  <si>
+    <t>Create UCS for UC "build towers on selected area"</t>
+  </si>
+  <si>
+    <t>DHTD-47</t>
+  </si>
+  <si>
+    <t>Create UCS for UC "Return to main menu"</t>
+  </si>
+  <si>
+    <t>DHTD-54</t>
+  </si>
+  <si>
+    <t>create handout for midterm presentation</t>
+  </si>
+  <si>
+    <t>DHTD-53</t>
+  </si>
+  <si>
+    <t>create the presentation for midterm exam</t>
+  </si>
+  <si>
+    <t>DHTD-51</t>
+  </si>
+  <si>
+    <t>Blog Entry Week 10</t>
+  </si>
+  <si>
+    <t>DHTD-52</t>
+  </si>
+  <si>
+    <t>Write Comments to other groups (Week 10)</t>
   </si>
 </sst>
 </file>
@@ -352,12 +406,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF33CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3300"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="20">
@@ -366,43 +444,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -418,117 +459,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -589,78 +519,352 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+      <color rgb="FFFF33CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -809,6 +1013,62 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>TicketLog3rdS!$L$2:$L$4</c:f>
@@ -833,13 +1093,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>45.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>44.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>70.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -998,6 +1258,82 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-76AB-4824-94A0-5ABDB7162347}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF33CC"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-76AB-4824-94A0-5ABDB7162347}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF3300"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-76AB-4824-94A0-5ABDB7162347}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-76AB-4824-94A0-5ABDB7162347}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>TicketLog3rdS!$N$1:$Q$1</c:f>
@@ -1025,16 +1361,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1155,16 +1491,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1223,6 +1559,13 @@
     <c:showDLblsOverMax val="0"/>
     <c:extLst/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -1323,7 +1666,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FFFF00"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1343,7 +1686,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF33CC"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1363,7 +1706,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="FF3300"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1383,7 +1726,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1398,6 +1741,62 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>TicketLog3rdS!$N$1:$Q$1</c:f>
@@ -1425,16 +1824,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>13.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>21.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1512,10 +1911,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="accent1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1621,7 +2017,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FFFF00"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1641,7 +2037,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF33CC"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1661,7 +2057,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="FF3300"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1681,7 +2077,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1696,6 +2092,62 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>TicketLog3rdS!$N$1:$Q$1</c:f>
@@ -1723,16 +2175,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>30.66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>15.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>15.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>8.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1810,10 +2262,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="accent1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1876,7 +2325,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" baseline="0"/>
-              <a:t> Type</a:t>
+              <a:t> Type (h)</a:t>
             </a:r>
             <a:endParaRPr lang="de-DE"/>
           </a:p>
@@ -1924,7 +2373,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FFFF00"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1944,7 +2393,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF33CC"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1964,7 +2413,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="FF3300"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1984,7 +2433,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1999,6 +2448,63 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>TicketLog3rdS!$L$8:$L$11</c:f>
@@ -2026,16 +2532,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>51.16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>42.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2113,10 +2619,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="accent1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -4824,7 +5327,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4841,1478 +5344,1915 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="P1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="Q1" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="Q1" s="29" t="s">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20">
+        <v>2</v>
+      </c>
+      <c r="G2" s="20">
+        <v>1.91</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="22">
+        <v>1.75</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="5">
+        <f>SUM(N2:Q2)</f>
+        <v>45.75</v>
+      </c>
+      <c r="N2" s="5">
+        <f>SUM(I30,I35,I55,I79)</f>
+        <v>7.25</v>
+      </c>
+      <c r="O2" s="5">
+        <f>SUM(I8,I11,I14,I21,I24,I59)</f>
+        <v>5.75</v>
+      </c>
+      <c r="P2" s="5">
+        <f>SUM(I33,I37,I38,I62,I65,I68)</f>
+        <v>26</v>
+      </c>
+      <c r="Q2" s="5">
+        <f>SUM(I27,I50,I53)</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="23"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="26">
+        <v>0.16</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="3">
+        <f>SUM(N3:Q3)</f>
+        <v>44.75</v>
+      </c>
+      <c r="N3" s="3">
+        <f>SUM(I7,I17,I26,I29,I41,I56,I58,I76,I78,I81)</f>
+        <v>13.25</v>
+      </c>
+      <c r="O3" s="3">
+        <f>SUM(I4,I10,I13,I20,I23,I43,I48,I49,I60,I72,I74)</f>
+        <v>21.25</v>
+      </c>
+      <c r="P3" s="3">
+        <f>SUM(I40,I46,I64,I67,I70)</f>
+        <v>6.75</v>
+      </c>
+      <c r="Q3" s="3">
+        <f>SUM(I28,I52)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28">
+        <v>8</v>
+      </c>
+      <c r="G4" s="28">
+        <v>3.75</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="30">
+        <v>3.75</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="3">
+        <f>SUM(N4:Q4)</f>
+        <v>70.91</v>
+      </c>
+      <c r="N4" s="3">
+        <f>SUM(I2,I3,I5,I6,I16,I18,I25,I31,I32,I34,I44,I45,I57,I75,I77,I80)</f>
+        <v>30.66</v>
+      </c>
+      <c r="O4" s="3">
+        <f>SUM(I9,I12,I15,I19,I22,I42,I61,I71,I73)</f>
+        <v>15.75</v>
+      </c>
+      <c r="P4" s="3">
+        <f>SUM(I36,I39,I47,I63,I66,I69)</f>
+        <v>15.75</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>SUM(I51,I54)</f>
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32">
+        <v>1</v>
+      </c>
+      <c r="G5" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="G6" s="32">
+        <v>1.25</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="34">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32">
+        <v>1</v>
+      </c>
+      <c r="G7" s="32">
+        <v>1</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="34">
+        <v>1</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36">
+        <v>6</v>
+      </c>
+      <c r="G8" s="36">
+        <v>6</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="38">
+        <v>2</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="5">
+        <f>SUM(N2:N4)</f>
+        <v>51.16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="42">
+        <v>4</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="3">
+        <f>SUM(O2:O4)</f>
+        <v>42.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="36">
+        <v>8</v>
+      </c>
+      <c r="G10" s="36">
+        <v>7</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="38">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M10" s="3">
+        <f>SUM(P2:P4)</f>
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="43"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="44">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="3">
+        <f>SUM(Q2:Q4)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="43"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="44">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="43"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="43"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="44">
+        <v>1</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="39"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="42">
+        <v>1.5</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="5">
+        <f>SUM(I10,I11,I12,I19,I20,I21,I33,I38,I39,I40,I50,I51)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="G16" s="32">
+        <v>1</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="34">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="3">
+        <f>SUM(I13,I14,I15,I22,I23,I24,I68,I69,I70)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32">
+        <v>1</v>
+      </c>
+      <c r="G17" s="32">
+        <v>1</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="34">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M17" s="3">
+        <f>SUM(I62,I63,I64,I65,I66,I67,I71,I72)</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32">
+        <v>2</v>
+      </c>
+      <c r="G18" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="34">
+        <v>1.5</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M18" s="3">
+        <f>SUM(I73,I74)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="36">
+        <v>2</v>
+      </c>
+      <c r="G19" s="36">
+        <v>3</v>
+      </c>
+      <c r="H19" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="43"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="44">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="43"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="44">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="43"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="44">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="43"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="44">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="39"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20">
+        <v>1</v>
+      </c>
+      <c r="G25" s="20">
+        <v>1</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="23"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46">
+        <v>4</v>
+      </c>
+      <c r="G27" s="46">
+        <v>4.25</v>
+      </c>
+      <c r="H27" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="49"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="52">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32">
+        <v>1</v>
+      </c>
+      <c r="G29" s="32">
+        <v>1</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G30" s="20">
+        <v>2.25</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="22">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="26">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32">
+        <v>8</v>
+      </c>
+      <c r="G32" s="32">
+        <v>6</v>
+      </c>
+      <c r="H32" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="54">
+        <v>8</v>
+      </c>
+      <c r="G33" s="54">
+        <v>6</v>
+      </c>
+      <c r="H33" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="I33" s="56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G34" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58">
+        <v>16</v>
+      </c>
+      <c r="G36" s="58">
+        <v>15.5</v>
+      </c>
+      <c r="H36" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="60">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="61"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="I37" s="64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" s="58">
+        <v>12</v>
+      </c>
+      <c r="G38" s="58">
+        <v>17</v>
+      </c>
+      <c r="H38" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="60">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="65"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I39" s="66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="61"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="I40" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32">
+        <v>2</v>
+      </c>
+      <c r="G41" s="32">
+        <v>1</v>
+      </c>
+      <c r="H41" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I41" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36">
+        <v>4</v>
+      </c>
+      <c r="G42" s="36">
+        <v>4</v>
+      </c>
+      <c r="H42" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="I42" s="38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40">
+        <v>4</v>
+      </c>
+      <c r="G43" s="40">
+        <v>3.5</v>
+      </c>
+      <c r="H43" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="I43" s="42">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20">
+        <v>1</v>
+      </c>
+      <c r="G44" s="20">
+        <v>2</v>
+      </c>
+      <c r="H44" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I44" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24">
+        <v>1</v>
+      </c>
+      <c r="G45" s="24">
+        <v>1</v>
+      </c>
+      <c r="H45" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="I45" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58">
+        <v>4</v>
+      </c>
+      <c r="G46" s="58">
+        <v>3.5</v>
+      </c>
+      <c r="H46" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I46" s="60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="61"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="62"/>
+      <c r="F47" s="62"/>
+      <c r="G47" s="62"/>
+      <c r="H47" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" s="64">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28">
+        <v>2</v>
+      </c>
+      <c r="G48" s="28">
+        <v>2</v>
+      </c>
+      <c r="H48" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I48" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="67" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="D49" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" s="68"/>
+      <c r="F49" s="68">
+        <v>8</v>
+      </c>
+      <c r="G49" s="68">
+        <v>8</v>
+      </c>
+      <c r="H49" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="I49" s="70">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="C50" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="E50" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="F50" s="46">
+        <v>8</v>
+      </c>
+      <c r="G50" s="46">
+        <v>11</v>
+      </c>
+      <c r="H50" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="I50" s="48">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="49"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" s="52">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="E52" s="46"/>
+      <c r="F52" s="46">
+        <v>5</v>
+      </c>
+      <c r="G52" s="46">
+        <v>3.75</v>
+      </c>
+      <c r="H52" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="I52" s="48">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="71"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I53" s="72">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="49"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="51"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="50"/>
+      <c r="H54" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="I54" s="52">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20">
+        <v>3</v>
+      </c>
+      <c r="G55" s="20">
+        <v>4</v>
+      </c>
+      <c r="H55" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I55" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="73"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="23"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
+      <c r="H57" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="E58" s="32"/>
+      <c r="F58" s="32">
+        <v>1</v>
+      </c>
+      <c r="G58" s="32">
+        <v>1</v>
+      </c>
+      <c r="H58" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I58" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="E59" s="36"/>
+      <c r="F59" s="36">
+        <v>3</v>
+      </c>
+      <c r="G59" s="36">
+        <v>2</v>
+      </c>
+      <c r="H59" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="I59" s="38">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="43"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I60" s="44">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="39"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="41"/>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="40"/>
+      <c r="H61" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="I61" s="42">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="57" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="B62" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C62" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" s="59" t="s">
+        <v>97</v>
+      </c>
+      <c r="E62" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="F62" s="58">
+        <v>2</v>
+      </c>
+      <c r="G62" s="58">
+        <v>2.5</v>
+      </c>
+      <c r="H62" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="I62" s="60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="65"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I63" s="66">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="61"/>
+      <c r="B64" s="62"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="63"/>
+      <c r="E64" s="62"/>
+      <c r="F64" s="62"/>
+      <c r="G64" s="62"/>
+      <c r="H64" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="I64" s="64">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B65" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C65" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="D65" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="E65" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="F65" s="58">
+        <v>2</v>
+      </c>
+      <c r="G65" s="58">
+        <v>2</v>
+      </c>
+      <c r="H65" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="I65" s="60">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="65"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I66" s="66">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="61"/>
+      <c r="B67" s="62"/>
+      <c r="C67" s="62"/>
+      <c r="D67" s="63"/>
+      <c r="E67" s="62"/>
+      <c r="F67" s="62"/>
+      <c r="G67" s="62"/>
+      <c r="H67" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="I67" s="64">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="B68" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C68" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="D68" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="E68" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="F68" s="58">
+        <v>2</v>
+      </c>
+      <c r="G68" s="58">
+        <v>2</v>
+      </c>
+      <c r="H68" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="I68" s="60">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="65"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I69" s="66">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="61"/>
+      <c r="B70" s="62"/>
+      <c r="C70" s="62"/>
+      <c r="D70" s="63"/>
+      <c r="E70" s="62"/>
+      <c r="F70" s="62"/>
+      <c r="G70" s="62"/>
+      <c r="H70" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="I70" s="64">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B71" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="E71" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="F71" s="36">
+        <v>3</v>
+      </c>
+      <c r="G71" s="36">
+        <v>2</v>
+      </c>
+      <c r="H71" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="I71" s="38">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="39"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="40"/>
+      <c r="D72" s="41"/>
+      <c r="E72" s="40"/>
+      <c r="F72" s="40"/>
+      <c r="G72" s="40"/>
+      <c r="H72" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="I72" s="42">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B73" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="E73" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="F73" s="36">
+        <v>2</v>
+      </c>
+      <c r="G73" s="36">
+        <v>1.5</v>
+      </c>
+      <c r="H73" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="I73" s="38">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="39"/>
+      <c r="B74" s="40"/>
+      <c r="C74" s="40"/>
+      <c r="D74" s="41"/>
+      <c r="E74" s="40"/>
+      <c r="F74" s="40"/>
+      <c r="G74" s="40"/>
+      <c r="H74" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="I74" s="42">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B75" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C75" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D75" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E75" s="20"/>
+      <c r="F75" s="20">
+        <v>4</v>
+      </c>
+      <c r="G75" s="20">
+        <v>3.5</v>
+      </c>
+      <c r="H75" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I75" s="22">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="23"/>
+      <c r="B76" s="24"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="24"/>
+      <c r="G76" s="24"/>
+      <c r="H76" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I76" s="26">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B77" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D77" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="E77" s="20"/>
+      <c r="F77" s="20">
         <v>15</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7">
-        <v>2</v>
-      </c>
-      <c r="G2" s="7">
-        <v>1.91</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="G77" s="20">
+        <v>12.25</v>
+      </c>
+      <c r="H77" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="9">
-        <v>1.75</v>
-      </c>
-      <c r="L2" s="24" t="s">
+      <c r="I77" s="22">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="73"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I78" s="74">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="23"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
+      <c r="H79" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="25">
-        <v>0</v>
-      </c>
-      <c r="N2" s="25">
-        <v>0</v>
-      </c>
-      <c r="O2" s="25">
-        <v>0</v>
-      </c>
-      <c r="P2" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11" t="s">
+      <c r="I79" s="26">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B80" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C80" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D80" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="E80" s="32"/>
+      <c r="F80" s="32">
+        <v>6</v>
+      </c>
+      <c r="G80" s="32">
+        <v>3.5</v>
+      </c>
+      <c r="H80" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="13">
-        <v>0.16</v>
-      </c>
-      <c r="L3" s="22" t="s">
+      <c r="I80" s="34">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B81" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D81" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="E81" s="32"/>
+      <c r="F81" s="32">
+        <v>1</v>
+      </c>
+      <c r="G81" s="32">
+        <v>1</v>
+      </c>
+      <c r="H81" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="23">
-        <v>0</v>
-      </c>
-      <c r="N3" s="23">
-        <v>0</v>
-      </c>
-      <c r="O3" s="23">
-        <v>0</v>
-      </c>
-      <c r="P3" s="23">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15">
-        <v>8</v>
-      </c>
-      <c r="G4" s="15">
-        <v>3.75</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="17">
-        <v>3.75</v>
-      </c>
-      <c r="L4" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="23">
-        <v>0</v>
-      </c>
-      <c r="N4" s="23">
-        <v>0</v>
-      </c>
-      <c r="O4" s="23">
-        <v>0</v>
-      </c>
-      <c r="P4" s="23">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15">
+      <c r="I81" s="34">
         <v>1</v>
-      </c>
-      <c r="G5" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="17">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15">
-        <v>1.5</v>
-      </c>
-      <c r="G6" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="17">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15">
-        <v>1</v>
-      </c>
-      <c r="G7" s="15">
-        <v>1</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="17">
-        <v>1</v>
-      </c>
-      <c r="L7" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="M7" s="29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7">
-        <v>6</v>
-      </c>
-      <c r="G8" s="7">
-        <v>6</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="9">
-        <v>2</v>
-      </c>
-      <c r="L8" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" s="25">
-        <f>SUM(N2:N4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="13">
-        <v>4</v>
-      </c>
-      <c r="L9" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="23">
-        <f>SUM(O2:O4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="7">
-        <v>8</v>
-      </c>
-      <c r="G10" s="7">
-        <v>7</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="9">
-        <v>1</v>
-      </c>
-      <c r="L10" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="M10" s="23">
-        <f>SUM(P2:P4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="21">
-        <v>1</v>
-      </c>
-      <c r="L11" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="23">
-        <f>SUM(Q2:Q4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="21">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="21">
-        <v>1</v>
-      </c>
-      <c r="L14" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="M14" s="29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="13">
-        <v>1.5</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="M15" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15">
-        <v>1.5</v>
-      </c>
-      <c r="G16" s="15">
-        <v>1</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="17">
-        <v>1</v>
-      </c>
-      <c r="L16" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="M16" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15">
-        <v>1</v>
-      </c>
-      <c r="G17" s="15">
-        <v>1</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="17">
-        <v>1</v>
-      </c>
-      <c r="L17" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="M17" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15">
-        <v>2</v>
-      </c>
-      <c r="G18" s="15">
-        <v>1.5</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="17">
-        <v>1.5</v>
-      </c>
-      <c r="L18" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="M18" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="7">
-        <v>2</v>
-      </c>
-      <c r="G19" s="7">
-        <v>3</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I20" s="21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I21" s="21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" s="21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I23" s="21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7">
-        <v>1</v>
-      </c>
-      <c r="G25" s="7">
-        <v>1</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I26" s="13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7">
-        <v>4</v>
-      </c>
-      <c r="G27" s="7">
-        <v>4.25</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I28" s="13">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15">
-        <v>1</v>
-      </c>
-      <c r="G29" s="15">
-        <v>1</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I29" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="G30" s="7">
-        <v>2.25</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="9">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I31" s="13">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15">
-        <v>8</v>
-      </c>
-      <c r="G32" s="15">
-        <v>6</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I32" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F33" s="15">
-        <v>8</v>
-      </c>
-      <c r="G33" s="15">
-        <v>6</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="I33" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="G34" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I34" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7">
-        <v>16</v>
-      </c>
-      <c r="G36" s="7">
-        <v>15.5</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I36" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I37" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F38" s="7">
-        <v>12</v>
-      </c>
-      <c r="G38" s="7">
-        <v>17</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" s="9">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="18"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="I39" s="21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I40" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15">
-        <v>2</v>
-      </c>
-      <c r="G41" s="15">
-        <v>1</v>
-      </c>
-      <c r="H41" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I41" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15">
-        <v>4</v>
-      </c>
-      <c r="G42" s="15">
-        <v>4</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I42" s="17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15">
-        <v>4</v>
-      </c>
-      <c r="G43" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I43" s="17">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15">
-        <v>1</v>
-      </c>
-      <c r="G44" s="15">
-        <v>2</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I44" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15">
-        <v>1</v>
-      </c>
-      <c r="G45" s="15">
-        <v>1</v>
-      </c>
-      <c r="H45" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I45" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7">
-        <v>4</v>
-      </c>
-      <c r="G46" s="7">
-        <v>3.5</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I46" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="10"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I47" s="13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15">
-        <v>2</v>
-      </c>
-      <c r="G48" s="15">
-        <v>2</v>
-      </c>
-      <c r="H48" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I48" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15">
-        <v>8</v>
-      </c>
-      <c r="G49" s="15">
-        <v>8</v>
-      </c>
-      <c r="H49" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I49" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F50" s="7">
-        <v>8</v>
-      </c>
-      <c r="G50" s="7">
-        <v>11</v>
-      </c>
-      <c r="H50" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I50" s="9">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="10"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I51" s="13">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7">
-        <v>5</v>
-      </c>
-      <c r="G52" s="7">
-        <v>3.75</v>
-      </c>
-      <c r="H52" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I52" s="9">
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="18"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I53" s="21">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="10"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I54" s="13">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7">
-        <v>3</v>
-      </c>
-      <c r="G55" s="7">
-        <v>4</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I55" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="18"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I56" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="10"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I57" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15">
-        <v>1</v>
-      </c>
-      <c r="G58" s="15">
-        <v>1</v>
-      </c>
-      <c r="H58" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I58" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E59" s="7"/>
-      <c r="F59" s="7">
-        <v>3</v>
-      </c>
-      <c r="G59" s="7">
-        <v>2</v>
-      </c>
-      <c r="H59" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I59" s="9">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="18"/>
-      <c r="B60" s="19"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I60" s="21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="10"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I61" s="13">
-        <v>0.75</v>
       </c>
     </row>
   </sheetData>
@@ -6326,9 +7266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D844987-9B48-4B0E-8368-94B59980651E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
[DHTD-68] Added UC-overview table
</commit_message>
<xml_diff>
--- a/midterm-presentation/TimeSheet.xlsx
+++ b/midterm-presentation/TimeSheet.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TowerDefense\midterm-presentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programmierung\Android\Tower-Defense\midterm-presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316F7735-7217-47D9-85CF-460B57F5CBBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19B5D60-2EE6-48B8-9164-906055AC4A60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="15960" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TicketLog3rdS" sheetId="1" r:id="rId1"/>
     <sheet name="Charts3rdS" sheetId="2" r:id="rId2"/>
+    <sheet name="Use Case Overview" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="130">
   <si>
     <t>Ticketart</t>
   </si>
@@ -389,13 +390,46 @@
   </si>
   <si>
     <t>Create Home activity</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>UC description</t>
+  </si>
+  <si>
+    <t>Documentation (h)</t>
+  </si>
+  <si>
+    <t>Coding (h)</t>
+  </si>
+  <si>
+    <t>Warm-Up time (h)</t>
+  </si>
+  <si>
+    <t>Total (h)</t>
+  </si>
+  <si>
+    <t>start the game from the menu*</t>
+  </si>
+  <si>
+    <t>*start the game from the menu:</t>
+  </si>
+  <si>
+    <t>This Use Case includes the implementation of the gameengine in order to have a base for playing the game</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,6 +447,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -751,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -903,6 +952,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -5379,21 +5431,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="39.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
-    <col min="9" max="9" width="20.77734375" customWidth="1"/>
-    <col min="12" max="17" width="17.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="39.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.08984375" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1"/>
+    <col min="9" max="9" width="20.81640625" customWidth="1"/>
+    <col min="12" max="17" width="17.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="75" t="s">
         <v>2</v>
       </c>
@@ -5440,7 +5494,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="83" t="s">
         <v>116</v>
       </c>
@@ -5490,7 +5544,7 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="87" t="s">
         <v>115</v>
       </c>
@@ -5542,7 +5596,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="79" t="s">
         <v>7</v>
       </c>
@@ -5592,7 +5646,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="23"/>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
@@ -5607,7 +5661,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="27" t="s">
         <v>8</v>
       </c>
@@ -5634,7 +5688,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="31" t="s">
         <v>9</v>
       </c>
@@ -5661,7 +5715,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="31" t="s">
         <v>10</v>
       </c>
@@ -5688,7 +5742,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="31" t="s">
         <v>11</v>
       </c>
@@ -5721,7 +5775,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>12</v>
       </c>
@@ -5755,7 +5809,7 @@
         <v>51.16</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="39"/>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>
@@ -5777,7 +5831,7 @@
         <v>52.75</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="35" t="s">
         <v>13</v>
       </c>
@@ -5813,7 +5867,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="43"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -5835,7 +5889,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="43"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -5850,7 +5904,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="43"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -5867,7 +5921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="43"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -5888,7 +5942,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="39"/>
       <c r="B17" s="40"/>
       <c r="C17" s="40"/>
@@ -5910,7 +5964,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="31" t="s">
         <v>32</v>
       </c>
@@ -5944,7 +5998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="31" t="s">
         <v>34</v>
       </c>
@@ -5978,7 +6032,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="31" t="s">
         <v>36</v>
       </c>
@@ -6012,7 +6066,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="35" t="s">
         <v>38</v>
       </c>
@@ -6041,7 +6095,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="43"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -6056,7 +6110,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="43"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -6071,7 +6125,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="43"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -6088,7 +6142,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="43"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -6103,7 +6157,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="39"/>
       <c r="B26" s="40"/>
       <c r="C26" s="40"/>
@@ -6118,7 +6172,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="19" t="s">
         <v>40</v>
       </c>
@@ -6145,7 +6199,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="23"/>
       <c r="B28" s="24"/>
       <c r="C28" s="24"/>
@@ -6160,7 +6214,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="45" t="s">
         <v>42</v>
       </c>
@@ -6187,7 +6241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="49"/>
       <c r="B30" s="50"/>
       <c r="C30" s="50"/>
@@ -6202,7 +6256,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="31" t="s">
         <v>45</v>
       </c>
@@ -6229,7 +6283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="19" t="s">
         <v>47</v>
       </c>
@@ -6256,7 +6310,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="23"/>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
@@ -6271,7 +6325,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="31" t="s">
         <v>49</v>
       </c>
@@ -6298,7 +6352,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="53" t="s">
         <v>51</v>
       </c>
@@ -6327,7 +6381,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="19" t="s">
         <v>54</v>
       </c>
@@ -6354,7 +6408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="23"/>
       <c r="B37" s="24"/>
       <c r="C37" s="24"/>
@@ -6369,7 +6423,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="57" t="s">
         <v>56</v>
       </c>
@@ -6396,7 +6450,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="61"/>
       <c r="B39" s="62"/>
       <c r="C39" s="62"/>
@@ -6411,7 +6465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="57" t="s">
         <v>59</v>
       </c>
@@ -6440,7 +6494,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="65"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -6455,7 +6509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="61"/>
       <c r="B42" s="62"/>
       <c r="C42" s="62"/>
@@ -6470,7 +6524,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="31" t="s">
         <v>61</v>
       </c>
@@ -6497,7 +6551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="35" t="s">
         <v>63</v>
       </c>
@@ -6524,7 +6578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="39" t="s">
         <v>65</v>
       </c>
@@ -6551,7 +6605,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="19" t="s">
         <v>67</v>
       </c>
@@ -6578,7 +6632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="23" t="s">
         <v>69</v>
       </c>
@@ -6605,7 +6659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="57" t="s">
         <v>71</v>
       </c>
@@ -6632,7 +6686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="61"/>
       <c r="B49" s="62"/>
       <c r="C49" s="62"/>
@@ -6647,7 +6701,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="27" t="s">
         <v>73</v>
       </c>
@@ -6674,7 +6728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="67" t="s">
         <v>75</v>
       </c>
@@ -6701,7 +6755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="45" t="s">
         <v>77</v>
       </c>
@@ -6730,7 +6784,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="49"/>
       <c r="B53" s="50"/>
       <c r="C53" s="50"/>
@@ -6745,7 +6799,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="45" t="s">
         <v>79</v>
       </c>
@@ -6772,7 +6826,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="71"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
@@ -6787,7 +6841,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="49"/>
       <c r="B56" s="50"/>
       <c r="C56" s="50"/>
@@ -6802,7 +6856,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="19" t="s">
         <v>81</v>
       </c>
@@ -6829,7 +6883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="73"/>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
@@ -6844,7 +6898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="23"/>
       <c r="B59" s="24"/>
       <c r="C59" s="24"/>
@@ -6859,7 +6913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="31" t="s">
         <v>83</v>
       </c>
@@ -6886,7 +6940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="35" t="s">
         <v>85</v>
       </c>
@@ -6913,7 +6967,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="43"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -6928,7 +6982,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="39"/>
       <c r="B63" s="40"/>
       <c r="C63" s="40"/>
@@ -6943,7 +6997,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="57" t="s">
         <v>96</v>
       </c>
@@ -6972,7 +7026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="65"/>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
@@ -6987,7 +7041,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="61"/>
       <c r="B66" s="62"/>
       <c r="C66" s="62"/>
@@ -7002,7 +7056,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="57" t="s">
         <v>99</v>
       </c>
@@ -7031,7 +7085,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="65"/>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>
@@ -7046,7 +7100,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="61"/>
       <c r="B69" s="62"/>
       <c r="C69" s="62"/>
@@ -7061,7 +7115,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="57" t="s">
         <v>101</v>
       </c>
@@ -7090,7 +7144,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="65"/>
       <c r="B71" s="17"/>
       <c r="C71" s="17"/>
@@ -7105,7 +7159,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="61"/>
       <c r="B72" s="62"/>
       <c r="C72" s="62"/>
@@ -7120,7 +7174,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A73" s="35" t="s">
         <v>103</v>
       </c>
@@ -7149,7 +7203,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="39"/>
       <c r="B74" s="40"/>
       <c r="C74" s="40"/>
@@ -7164,7 +7218,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="35" t="s">
         <v>105</v>
       </c>
@@ -7193,7 +7247,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="39"/>
       <c r="B76" s="40"/>
       <c r="C76" s="40"/>
@@ -7208,7 +7262,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="19" t="s">
         <v>107</v>
       </c>
@@ -7235,7 +7289,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="23"/>
       <c r="B78" s="24"/>
       <c r="C78" s="24"/>
@@ -7250,7 +7304,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="19" t="s">
         <v>109</v>
       </c>
@@ -7277,7 +7331,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="73"/>
       <c r="B80" s="11"/>
       <c r="C80" s="11"/>
@@ -7292,7 +7346,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="23"/>
       <c r="B81" s="24"/>
       <c r="C81" s="24"/>
@@ -7307,7 +7361,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="31" t="s">
         <v>111</v>
       </c>
@@ -7334,7 +7388,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="31" t="s">
         <v>113</v>
       </c>
@@ -7374,12 +7428,186 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.90625" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C55BAC4-B6C8-4445-BEEB-A5DE06A20711}">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="31.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" customWidth="1"/>
+    <col min="6" max="6" width="16" style="93" customWidth="1"/>
+    <col min="9" max="9" width="11.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="91" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="91" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="91" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="91" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="92" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="91" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="91"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2">
+        <f>3.5+1.5</f>
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <f>4+6+17</f>
+        <v>27</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2" s="93">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <f>3.5+1.5</f>
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="93">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>7.5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f>4.5</f>
+        <v>4.5</v>
+      </c>
+      <c r="E4">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="93">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>6.5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5">
+        <f>1.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="D5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="93">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1.5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="91" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[DHTD-76] Use Case Overview Table updated
</commit_message>
<xml_diff>
--- a/midterm-presentation/TimeSheet.xlsx
+++ b/midterm-presentation/TimeSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programmierung\Android\Tower-Defense\midterm-presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19B5D60-2EE6-48B8-9164-906055AC4A60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D65B5D7-172E-4C4C-902A-61DF76885A0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15960" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TicketLog3rdS" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="129">
   <si>
     <t>Ticketart</t>
   </si>
@@ -413,16 +413,13 @@
     <t>Total (h)</t>
   </si>
   <si>
-    <t>start the game from the menu*</t>
-  </si>
-  <si>
-    <t>*start the game from the menu:</t>
-  </si>
-  <si>
-    <t>This Use Case includes the implementation of the gameengine in order to have a base for playing the game</t>
-  </si>
-  <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>GameEngine - Foundation</t>
+  </si>
+  <si>
+    <t>---</t>
   </si>
 </sst>
 </file>
@@ -800,7 +797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -955,6 +952,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -5431,7 +5430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
@@ -7480,106 +7479,109 @@
       <c r="I1" s="91"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2">
-        <f>3.5+1.5</f>
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <f>4+6+17</f>
-        <v>27</v>
-      </c>
-      <c r="E2">
-        <v>8</v>
+      <c r="A2" s="94">
+        <v>0</v>
+      </c>
+      <c r="B2" s="94" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="94">
+        <v>0</v>
+      </c>
+      <c r="D2" s="94">
+        <f>6+15.5+17+3.5</f>
+        <v>42</v>
+      </c>
+      <c r="E2" s="94">
+        <f>3.75+4.25+1</f>
+        <v>9</v>
       </c>
       <c r="F2" s="93">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>40</v>
-      </c>
-      <c r="H2" t="s">
-        <v>129</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G2" s="94">
+        <f>C2+D2+E2</f>
+        <v>51</v>
+      </c>
+      <c r="H2" s="95" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="91"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <f>3.5+1.5</f>
         <v>5</v>
       </c>
       <c r="D3">
+        <f>4</f>
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f>3</f>
+        <v>3</v>
+      </c>
+      <c r="F3" s="93">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <f>C3+D3+E3</f>
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <f>3.5+1.5</f>
+        <v>5</v>
+      </c>
+      <c r="D4">
         <f>2</f>
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>0.5</v>
-      </c>
-      <c r="F3" s="93">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>7.5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4">
-        <f>2</f>
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <f>4.5</f>
-        <v>4.5</v>
-      </c>
-      <c r="E4">
-        <f>0</f>
-        <v>0</v>
       </c>
       <c r="F4" s="93">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <v>6.5</v>
+        <f>C4+D4+E4</f>
+        <v>7.5</v>
       </c>
       <c r="H4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C5">
-        <f>1.5</f>
-        <v>1.5</v>
+        <f>2</f>
+        <v>2</v>
       </c>
       <c r="D5">
-        <f>0</f>
-        <v>0</v>
+        <f>4.5</f>
+        <v>4.5</v>
       </c>
       <c r="E5">
         <f>0</f>
@@ -7590,21 +7592,46 @@
         <v>0</v>
       </c>
       <c r="G5">
+        <f>C5+D5+E5</f>
+        <v>6.5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6">
+        <f>1.5</f>
         <v>1.5</v>
       </c>
-      <c r="H5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="91" t="s">
-        <v>127</v>
+      <c r="D6">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="93">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f>C6+D6+E6</f>
+        <v>1.5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>128</v>
-      </c>
+      <c r="A22" s="91"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[DHTD-77] Function Point Calculation and Overview
</commit_message>
<xml_diff>
--- a/midterm-presentation/TimeSheet.xlsx
+++ b/midterm-presentation/TimeSheet.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programmierung\Android\Tower-Defense\midterm-presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D65B5D7-172E-4C4C-902A-61DF76885A0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA378C5-34A3-46C0-ACD9-6FCE92936472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TicketLog3rdS" sheetId="1" r:id="rId1"/>
     <sheet name="Charts3rdS" sheetId="2" r:id="rId2"/>
     <sheet name="Use Case Overview" sheetId="3" r:id="rId3"/>
+    <sheet name="FP Calculation" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="224">
   <si>
     <t>Ticketart</t>
   </si>
@@ -420,13 +421,298 @@
   </si>
   <si>
     <t>---</t>
+  </si>
+  <si>
+    <t>Upgrade Towers</t>
+  </si>
+  <si>
+    <t>Sell Towers</t>
+  </si>
+  <si>
+    <t>Select between different Towers</t>
+  </si>
+  <si>
+    <t>Edit Settings</t>
+  </si>
+  <si>
+    <t>Toggle Sound &amp; Animations</t>
+  </si>
+  <si>
+    <t>Choose Difficulties</t>
+  </si>
+  <si>
+    <t>RET</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>FTR</t>
+  </si>
+  <si>
+    <t>Complexity</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>RETs</t>
+  </si>
+  <si>
+    <t>DETs</t>
+  </si>
+  <si>
+    <t>FTRs</t>
+  </si>
+  <si>
+    <t>UC1: Start the game from the menu</t>
+  </si>
+  <si>
+    <t>External Inputs</t>
+  </si>
+  <si>
+    <t>External Outputs</t>
+  </si>
+  <si>
+    <t>External Queries</t>
+  </si>
+  <si>
+    <t>Internal Logical Files</t>
+  </si>
+  <si>
+    <t>External Interface Files</t>
+  </si>
+  <si>
+    <t>Function Points</t>
+  </si>
+  <si>
+    <t>UC2: Start Waves</t>
+  </si>
+  <si>
+    <t>UC3: Build Towers on selected Area</t>
+  </si>
+  <si>
+    <t>UC4: Return to main menu</t>
+  </si>
+  <si>
+    <t>UC5: Upgrade Towers</t>
+  </si>
+  <si>
+    <t>UC6: Sell Towers</t>
+  </si>
+  <si>
+    <t>UC7: Select between different Towers</t>
+  </si>
+  <si>
+    <t>UC8: Edit Settings</t>
+  </si>
+  <si>
+    <t>UC9: Toggle Sound &amp; Animations</t>
+  </si>
+  <si>
+    <t>UC10: Choose Difficulties</t>
+  </si>
+  <si>
+    <t>FP-Calculator:</t>
+  </si>
+  <si>
+    <t>http://groups.umd.umich.edu/cis/course.des/cis525/js/f00/harvey/FP_Calc.html?tCountVal=0#FPCalc</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>Complexity:</t>
+  </si>
+  <si>
+    <t>RET: Record Element Type</t>
+  </si>
+  <si>
+    <t>DET: Data Element Type</t>
+  </si>
+  <si>
+    <t>FTR: File Type Reference</t>
+  </si>
+  <si>
+    <t>GameActivity</t>
+  </si>
+  <si>
+    <t>Field-Buttons, Moving Tanks, generated Map</t>
+  </si>
+  <si>
+    <t>MainActivity</t>
+  </si>
+  <si>
+    <t>Tanks, Map</t>
+  </si>
+  <si>
+    <t>GameActivity, MapStructure, Game</t>
+  </si>
+  <si>
+    <t>wave-button</t>
+  </si>
+  <si>
+    <t>GameActivity, Game, MatchField</t>
+  </si>
+  <si>
+    <t>wave-button, Tanks</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>Game, MatchField</t>
+  </si>
+  <si>
+    <t>MatchField, Tower</t>
+  </si>
+  <si>
+    <t>Field-Buttons, Plus-Symbol</t>
+  </si>
+  <si>
+    <t>MatchField, Tower, Plus-Symbol</t>
+  </si>
+  <si>
+    <t>Main-Menu-Button, GameActivity</t>
+  </si>
+  <si>
+    <t>Play-Button, MainActivity</t>
+  </si>
+  <si>
+    <t>GameActivity, Game</t>
+  </si>
+  <si>
+    <t>Game, MatchField, Enemies</t>
+  </si>
+  <si>
+    <t>Game, MatchField, Enemies, Tanks, MapStructure</t>
+  </si>
+  <si>
+    <t>Tower, MatchField</t>
+  </si>
+  <si>
+    <t>Tanks, Map, Fields, MatchField, Game</t>
+  </si>
+  <si>
+    <t>Tower-Selection, Upgrade-Button</t>
+  </si>
+  <si>
+    <t>Tower, GameActivity</t>
+  </si>
+  <si>
+    <t>Tower-Stats</t>
+  </si>
+  <si>
+    <t>Tower</t>
+  </si>
+  <si>
+    <t>GameActivity, Tower, Upgrade-UI</t>
+  </si>
+  <si>
+    <t>Tower-Selection, Sell-Button</t>
+  </si>
+  <si>
+    <t>Tower, MatchField, GameActivity</t>
+  </si>
+  <si>
+    <t>GameActivity, Tower, Sell-UI</t>
+  </si>
+  <si>
+    <t>GameActivity, Tower, MatchField</t>
+  </si>
+  <si>
+    <t>GameActivity, Tower, Level-Constants</t>
+  </si>
+  <si>
+    <t>Tower, Position</t>
+  </si>
+  <si>
+    <t>Tower, Game</t>
+  </si>
+  <si>
+    <t>Tower-Selection, Select-Button</t>
+  </si>
+  <si>
+    <t>Money, Price</t>
+  </si>
+  <si>
+    <t>GameActivity, Game, Money</t>
+  </si>
+  <si>
+    <t>GameActivity, Game, Tower-Template</t>
+  </si>
+  <si>
+    <t>Menu-Button</t>
+  </si>
+  <si>
+    <t>Settings-UI</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>SharedPreferences</t>
+  </si>
+  <si>
+    <t>SharedPreferences, GameActivity, Game</t>
+  </si>
+  <si>
+    <t>Settings, GameActivity</t>
+  </si>
+  <si>
+    <t>Settings-Buttons</t>
+  </si>
+  <si>
+    <t>Settings-Buttons, changed Settings</t>
+  </si>
+  <si>
+    <t>Settings, GameActivity, MainActivity</t>
+  </si>
+  <si>
+    <t>SharedPreferences, GameActivity, MainActivity</t>
+  </si>
+  <si>
+    <t>MainActivity, Difficulty, Play-Button</t>
+  </si>
+  <si>
+    <t>GameActivity, Game, Game-Settings</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>SharedPreferences, MainActivity, GameActivity</t>
+  </si>
+  <si>
+    <t>Statistics, GameActivity, MainActivity</t>
+  </si>
+  <si>
+    <t>Estimation: 10,1h</t>
+  </si>
+  <si>
+    <t>Estimation: 9,86h</t>
+  </si>
+  <si>
+    <t>Estimation: 4,3h</t>
+  </si>
+  <si>
+    <t>Estimation: 6,4h</t>
+  </si>
+  <si>
+    <t>Estimation: 9,1h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,8 +749,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,8 +796,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -793,11 +1099,224 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -954,8 +1473,110 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="29" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="29" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Akzent3" xfId="1" builtinId="37"/>
+    <cellStyle name="Link" xfId="2" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2744,6 +3365,481 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.4914260717410336E-2"/>
+          <c:y val="0.17092165898617515"/>
+          <c:w val="0.90286351706036749"/>
+          <c:h val="0.72217388149062012"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Time spent</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.4327865266841645E-2"/>
+                  <c:y val="-0.14422076272723974"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Use Case Overview'!$G$3:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>82</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>81</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>64</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>44</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E5D7-466A-BCCE-279B40FDE66F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="638654784"/>
+        <c:axId val="638651504"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="638654784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Time spent</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="638651504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="638651504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Function Points</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="638654784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2904,6 +4000,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
@@ -4948,6 +6084,522 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5157,6 +6809,157 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1" descr="table">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7968B003-AB30-4A53-A748-0C4165D9144C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11156950" y="2317750"/>
+          <a:ext cx="4413250" cy="5384800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>9540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15E19CDA-CA7E-49B8-B62E-E6691C657EF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17897475" y="3352800"/>
+          <a:ext cx="5924550" cy="5584840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>88897</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>30160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Diagramm 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70942551-88FC-49C2-B255-6BEEDB049744}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7441,7 +9244,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C55BAC4-B6C8-4445-BEEB-A5DE06A20711}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -7630,6 +9435,54 @@
         <v>126</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>134</v>
+      </c>
+    </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="91"/>
     </row>
@@ -7637,4 +9490,2042 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3800D6FA-69EA-4E12-9E16-1909B3CAE7B3}">
+  <dimension ref="A1:Q89"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37.1796875" style="94" customWidth="1"/>
+    <col min="2" max="7" width="10.90625" style="101"/>
+    <col min="8" max="9" width="19.6328125" style="131" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" style="131" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="91" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="119" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="115" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="110"/>
+      <c r="H1" s="123" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" s="125" t="s">
+        <v>142</v>
+      </c>
+      <c r="M1" s="91" t="s">
+        <v>159</v>
+      </c>
+      <c r="O1" s="103" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="120" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="116" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="106">
+        <v>2</v>
+      </c>
+      <c r="D2" s="106">
+        <v>1</v>
+      </c>
+      <c r="E2" s="106" t="s">
+        <v>161</v>
+      </c>
+      <c r="F2" s="107">
+        <f>C2+D2</f>
+        <v>3</v>
+      </c>
+      <c r="G2" s="99"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="127" t="s">
+        <v>182</v>
+      </c>
+      <c r="J2" s="127" t="s">
+        <v>170</v>
+      </c>
+      <c r="M2" s="91" t="s">
+        <v>164</v>
+      </c>
+      <c r="O2" t="s">
+        <v>161</v>
+      </c>
+      <c r="P2" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="121" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="117" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="97">
+        <v>3</v>
+      </c>
+      <c r="D3" s="97">
+        <v>3</v>
+      </c>
+      <c r="E3" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F3" s="98">
+        <f t="shared" ref="F3:F4" si="0">C3+D3</f>
+        <v>6</v>
+      </c>
+      <c r="G3" s="99"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="128" t="s">
+        <v>169</v>
+      </c>
+      <c r="J3" s="128" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="97">
+        <v>0</v>
+      </c>
+      <c r="D4" s="97">
+        <v>0</v>
+      </c>
+      <c r="E4" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F4" s="98">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="99"/>
+      <c r="H4" s="126"/>
+      <c r="I4" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J4" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="M4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="121" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="100">
+        <v>2</v>
+      </c>
+      <c r="C5" s="97">
+        <v>5</v>
+      </c>
+      <c r="D5" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F5" s="98">
+        <f>B5+C5</f>
+        <v>7</v>
+      </c>
+      <c r="G5" s="99"/>
+      <c r="H5" s="129" t="s">
+        <v>171</v>
+      </c>
+      <c r="I5" s="128" t="s">
+        <v>187</v>
+      </c>
+      <c r="J5" s="126"/>
+      <c r="M5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="122" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="104">
+        <v>0</v>
+      </c>
+      <c r="C6" s="105">
+        <v>0</v>
+      </c>
+      <c r="D6" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="111">
+        <f>B6+C6</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="99"/>
+      <c r="H6" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J6" s="126"/>
+      <c r="M6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="119" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="112">
+        <v>82</v>
+      </c>
+      <c r="C7" s="112"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="130"/>
+    </row>
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="119" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="115" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="G10" s="110"/>
+      <c r="H10" s="123" t="s">
+        <v>140</v>
+      </c>
+      <c r="I10" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="J10" s="125" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="120" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="106">
+        <v>1</v>
+      </c>
+      <c r="D11" s="106">
+        <v>2</v>
+      </c>
+      <c r="E11" s="106" t="s">
+        <v>161</v>
+      </c>
+      <c r="F11" s="107">
+        <f>C11+D11</f>
+        <v>3</v>
+      </c>
+      <c r="G11" s="99"/>
+      <c r="H11" s="126"/>
+      <c r="I11" s="127" t="s">
+        <v>173</v>
+      </c>
+      <c r="J11" s="127" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="121" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="97">
+        <v>2</v>
+      </c>
+      <c r="D12" s="97">
+        <v>2</v>
+      </c>
+      <c r="E12" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F12" s="98">
+        <f t="shared" ref="F12:F13" si="1">C12+D12</f>
+        <v>4</v>
+      </c>
+      <c r="G12" s="99"/>
+      <c r="H12" s="126"/>
+      <c r="I12" s="128" t="s">
+        <v>175</v>
+      </c>
+      <c r="J12" s="128" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="97">
+        <v>0</v>
+      </c>
+      <c r="D13" s="97">
+        <v>0</v>
+      </c>
+      <c r="E13" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" s="98">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="99"/>
+      <c r="H13" s="126"/>
+      <c r="I13" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13" s="132" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="121" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="100">
+        <v>3</v>
+      </c>
+      <c r="C14" s="97">
+        <v>5</v>
+      </c>
+      <c r="D14" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" s="98">
+        <f>B14+C14</f>
+        <v>8</v>
+      </c>
+      <c r="G14" s="99"/>
+      <c r="H14" s="129" t="s">
+        <v>184</v>
+      </c>
+      <c r="I14" s="128" t="s">
+        <v>185</v>
+      </c>
+      <c r="J14" s="126"/>
+    </row>
+    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="122" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="104">
+        <v>0</v>
+      </c>
+      <c r="C15" s="105">
+        <v>0</v>
+      </c>
+      <c r="D15" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="F15" s="111">
+        <f>B15+C15</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="99"/>
+      <c r="H15" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="I15" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J15" s="126"/>
+    </row>
+    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="119" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="112">
+        <v>81</v>
+      </c>
+      <c r="C16" s="112"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="113"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="130"/>
+      <c r="I16" s="130"/>
+      <c r="J16" s="130"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="119" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" s="115" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="G19" s="110"/>
+      <c r="H19" s="123" t="s">
+        <v>140</v>
+      </c>
+      <c r="I19" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="J19" s="125" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="120" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="106">
+        <v>2</v>
+      </c>
+      <c r="D20" s="106">
+        <v>3</v>
+      </c>
+      <c r="E20" s="106" t="s">
+        <v>162</v>
+      </c>
+      <c r="F20" s="107">
+        <f>C20+D20</f>
+        <v>5</v>
+      </c>
+      <c r="G20" s="99"/>
+      <c r="H20" s="126"/>
+      <c r="I20" s="127" t="s">
+        <v>179</v>
+      </c>
+      <c r="J20" s="127" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="121" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="97">
+        <v>2</v>
+      </c>
+      <c r="D21" s="97">
+        <v>2</v>
+      </c>
+      <c r="E21" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F21" s="98">
+        <f t="shared" ref="F21:F22" si="2">C21+D21</f>
+        <v>4</v>
+      </c>
+      <c r="G21" s="99"/>
+      <c r="H21" s="126"/>
+      <c r="I21" s="128" t="s">
+        <v>186</v>
+      </c>
+      <c r="J21" s="128" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="97">
+        <v>0</v>
+      </c>
+      <c r="D22" s="97">
+        <v>0</v>
+      </c>
+      <c r="E22" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F22" s="98">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="99"/>
+      <c r="H22" s="126"/>
+      <c r="I22" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J22" s="132" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="121" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="100">
+        <v>2</v>
+      </c>
+      <c r="C23" s="97">
+        <v>2</v>
+      </c>
+      <c r="D23" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F23" s="98">
+        <f>B23+C23</f>
+        <v>4</v>
+      </c>
+      <c r="G23" s="99"/>
+      <c r="H23" s="129" t="s">
+        <v>177</v>
+      </c>
+      <c r="I23" s="128" t="s">
+        <v>177</v>
+      </c>
+      <c r="J23" s="126"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="122" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="104">
+        <v>0</v>
+      </c>
+      <c r="C24" s="105">
+        <v>0</v>
+      </c>
+      <c r="D24" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="F24" s="111">
+        <f>B24+C24</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="99"/>
+      <c r="H24" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="I24" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J24" s="126"/>
+    </row>
+    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="119" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" s="112">
+        <v>64</v>
+      </c>
+      <c r="C25" s="112"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="112"/>
+      <c r="F25" s="113"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="130"/>
+      <c r="I25" s="130"/>
+      <c r="J25" s="130"/>
+    </row>
+    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="119" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" s="115" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="G28" s="110"/>
+      <c r="H28" s="123" t="s">
+        <v>140</v>
+      </c>
+      <c r="I28" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="J28" s="125" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="120" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="106">
+        <v>2</v>
+      </c>
+      <c r="D29" s="106">
+        <v>2</v>
+      </c>
+      <c r="E29" s="106" t="s">
+        <v>161</v>
+      </c>
+      <c r="F29" s="107">
+        <f>C29+D29</f>
+        <v>4</v>
+      </c>
+      <c r="G29" s="99"/>
+      <c r="H29" s="126"/>
+      <c r="I29" s="127" t="s">
+        <v>181</v>
+      </c>
+      <c r="J29" s="127" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="121" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="97">
+        <v>1</v>
+      </c>
+      <c r="D30" s="97">
+        <v>0</v>
+      </c>
+      <c r="E30" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F30" s="98">
+        <f t="shared" ref="F30:F31" si="3">C30+D30</f>
+        <v>1</v>
+      </c>
+      <c r="G30" s="99"/>
+      <c r="H30" s="126"/>
+      <c r="I30" s="128" t="s">
+        <v>170</v>
+      </c>
+      <c r="J30" s="132" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="B31" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="97">
+        <v>0</v>
+      </c>
+      <c r="D31" s="97">
+        <v>0</v>
+      </c>
+      <c r="E31" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F31" s="98">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="99"/>
+      <c r="H31" s="126"/>
+      <c r="I31" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J31" s="132" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="121" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" s="100">
+        <v>2</v>
+      </c>
+      <c r="C32" s="97">
+        <v>2</v>
+      </c>
+      <c r="D32" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F32" s="98">
+        <f>B32+C32</f>
+        <v>4</v>
+      </c>
+      <c r="G32" s="99"/>
+      <c r="H32" s="129" t="s">
+        <v>183</v>
+      </c>
+      <c r="I32" s="128" t="s">
+        <v>183</v>
+      </c>
+      <c r="J32" s="126"/>
+    </row>
+    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="122" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" s="104">
+        <v>0</v>
+      </c>
+      <c r="C33" s="105">
+        <v>0</v>
+      </c>
+      <c r="D33" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="F33" s="111">
+        <f>B33+C33</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="99"/>
+      <c r="H33" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="I33" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J33" s="126"/>
+    </row>
+    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="119" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34" s="112">
+        <v>44</v>
+      </c>
+      <c r="C34" s="112"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="113"/>
+      <c r="G34" s="102"/>
+      <c r="H34" s="130"/>
+      <c r="I34" s="130"/>
+      <c r="J34" s="130"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G35" s="102"/>
+    </row>
+    <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G36" s="102"/>
+    </row>
+    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="119" t="s">
+        <v>153</v>
+      </c>
+      <c r="B37" s="115" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="D37" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="E37" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="G37" s="110"/>
+      <c r="H37" s="123" t="s">
+        <v>140</v>
+      </c>
+      <c r="I37" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="J37" s="125" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="120" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" s="106">
+        <v>2</v>
+      </c>
+      <c r="D38" s="106">
+        <v>2</v>
+      </c>
+      <c r="E38" s="106" t="s">
+        <v>161</v>
+      </c>
+      <c r="F38" s="107">
+        <f>C38+D38</f>
+        <v>4</v>
+      </c>
+      <c r="G38" s="99"/>
+      <c r="H38" s="126"/>
+      <c r="I38" s="127" t="s">
+        <v>188</v>
+      </c>
+      <c r="J38" s="127" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="121" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="97">
+        <v>3</v>
+      </c>
+      <c r="D39" s="97">
+        <v>2</v>
+      </c>
+      <c r="E39" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F39" s="98">
+        <f t="shared" ref="F39:F40" si="4">C39+D39</f>
+        <v>5</v>
+      </c>
+      <c r="G39" s="99"/>
+      <c r="H39" s="126"/>
+      <c r="I39" s="128" t="s">
+        <v>194</v>
+      </c>
+      <c r="J39" s="128" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A40" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="97">
+        <v>1</v>
+      </c>
+      <c r="D40" s="97">
+        <v>1</v>
+      </c>
+      <c r="E40" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F40" s="98">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G40" s="99"/>
+      <c r="H40" s="126"/>
+      <c r="I40" s="128" t="s">
+        <v>190</v>
+      </c>
+      <c r="J40" s="128" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="121" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="100">
+        <v>3</v>
+      </c>
+      <c r="C41" s="97">
+        <v>3</v>
+      </c>
+      <c r="D41" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E41" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F41" s="98">
+        <f>B41+C41</f>
+        <v>6</v>
+      </c>
+      <c r="G41" s="99"/>
+      <c r="H41" s="129" t="s">
+        <v>197</v>
+      </c>
+      <c r="I41" s="128" t="s">
+        <v>192</v>
+      </c>
+      <c r="J41" s="126"/>
+    </row>
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="122" t="s">
+        <v>148</v>
+      </c>
+      <c r="B42" s="104">
+        <v>0</v>
+      </c>
+      <c r="C42" s="105">
+        <v>0</v>
+      </c>
+      <c r="D42" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E42" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="F42" s="111">
+        <f>B42+C42</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="99"/>
+      <c r="H42" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="I42" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J42" s="126"/>
+      <c r="K42" s="96"/>
+    </row>
+    <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="119" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" s="112">
+        <v>80</v>
+      </c>
+      <c r="C43" s="112"/>
+      <c r="D43" s="112"/>
+      <c r="E43" s="112"/>
+      <c r="F43" s="113"/>
+      <c r="G43" s="102"/>
+      <c r="H43" s="130"/>
+      <c r="I43" s="130"/>
+      <c r="J43" s="130"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A44" s="133" t="s">
+        <v>219</v>
+      </c>
+      <c r="G44" s="102"/>
+    </row>
+    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G45" s="102"/>
+    </row>
+    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="119" t="s">
+        <v>154</v>
+      </c>
+      <c r="B46" s="115" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="F46" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="G46" s="110"/>
+      <c r="H46" s="123" t="s">
+        <v>140</v>
+      </c>
+      <c r="I46" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="J46" s="125" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A47" s="120" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" s="106">
+        <v>2</v>
+      </c>
+      <c r="D47" s="106">
+        <v>2</v>
+      </c>
+      <c r="E47" s="106" t="s">
+        <v>161</v>
+      </c>
+      <c r="F47" s="107">
+        <f>C47+D47</f>
+        <v>4</v>
+      </c>
+      <c r="G47" s="99"/>
+      <c r="H47" s="126"/>
+      <c r="I47" s="127" t="s">
+        <v>193</v>
+      </c>
+      <c r="J47" s="127" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" s="121" t="s">
+        <v>145</v>
+      </c>
+      <c r="B48" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" s="97">
+        <v>3</v>
+      </c>
+      <c r="D48" s="97">
+        <v>2</v>
+      </c>
+      <c r="E48" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F48" s="98">
+        <f t="shared" ref="F48:F49" si="5">C48+D48</f>
+        <v>5</v>
+      </c>
+      <c r="G48" s="99"/>
+      <c r="H48" s="126"/>
+      <c r="I48" s="128" t="s">
+        <v>194</v>
+      </c>
+      <c r="J48" s="128" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A49" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" s="97">
+        <v>1</v>
+      </c>
+      <c r="D49" s="97">
+        <v>1</v>
+      </c>
+      <c r="E49" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F49" s="98">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="G49" s="99"/>
+      <c r="H49" s="126"/>
+      <c r="I49" s="128" t="s">
+        <v>190</v>
+      </c>
+      <c r="J49" s="128" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A50" s="121" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" s="100">
+        <v>3</v>
+      </c>
+      <c r="C50" s="97">
+        <v>3</v>
+      </c>
+      <c r="D50" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F50" s="98">
+        <f>B50+C50</f>
+        <v>6</v>
+      </c>
+      <c r="G50" s="99"/>
+      <c r="H50" s="129" t="s">
+        <v>196</v>
+      </c>
+      <c r="I50" s="128" t="s">
+        <v>195</v>
+      </c>
+      <c r="J50" s="126"/>
+    </row>
+    <row r="51" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="122" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="104">
+        <v>0</v>
+      </c>
+      <c r="C51" s="105">
+        <v>0</v>
+      </c>
+      <c r="D51" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="F51" s="111">
+        <f>B51+C51</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="99"/>
+      <c r="H51" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="I51" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J51" s="126"/>
+    </row>
+    <row r="52" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="119" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" s="112">
+        <v>80</v>
+      </c>
+      <c r="C52" s="112"/>
+      <c r="D52" s="112"/>
+      <c r="E52" s="112"/>
+      <c r="F52" s="113"/>
+      <c r="G52" s="102"/>
+      <c r="H52" s="130"/>
+      <c r="I52" s="130"/>
+      <c r="J52" s="130"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A53" s="133" t="s">
+        <v>219</v>
+      </c>
+      <c r="G53" s="102"/>
+    </row>
+    <row r="54" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G54" s="102"/>
+    </row>
+    <row r="55" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="119" t="s">
+        <v>155</v>
+      </c>
+      <c r="B55" s="115" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="D55" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="E55" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="F55" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="G55" s="110"/>
+      <c r="H55" s="123" t="s">
+        <v>140</v>
+      </c>
+      <c r="I55" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="J55" s="125" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A56" s="120" t="s">
+        <v>144</v>
+      </c>
+      <c r="B56" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" s="106">
+        <v>2</v>
+      </c>
+      <c r="D56" s="106">
+        <v>2</v>
+      </c>
+      <c r="E56" s="106" t="s">
+        <v>161</v>
+      </c>
+      <c r="F56" s="107">
+        <f>C56+D56</f>
+        <v>4</v>
+      </c>
+      <c r="G56" s="99"/>
+      <c r="H56" s="126"/>
+      <c r="I56" s="127" t="s">
+        <v>198</v>
+      </c>
+      <c r="J56" s="127" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A57" s="121" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57" s="97">
+        <v>2</v>
+      </c>
+      <c r="D57" s="97">
+        <v>2</v>
+      </c>
+      <c r="E57" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F57" s="98">
+        <f t="shared" ref="F57:F58" si="6">C57+D57</f>
+        <v>4</v>
+      </c>
+      <c r="G57" s="99"/>
+      <c r="H57" s="126"/>
+      <c r="I57" s="128" t="s">
+        <v>200</v>
+      </c>
+      <c r="J57" s="128" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A58" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="B58" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C58" s="97">
+        <v>2</v>
+      </c>
+      <c r="D58" s="97">
+        <v>1</v>
+      </c>
+      <c r="E58" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F58" s="98">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="G58" s="99"/>
+      <c r="H58" s="126"/>
+      <c r="I58" s="128" t="s">
+        <v>201</v>
+      </c>
+      <c r="J58" s="128" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A59" s="121" t="s">
+        <v>147</v>
+      </c>
+      <c r="B59" s="100">
+        <v>3</v>
+      </c>
+      <c r="C59" s="97">
+        <v>3</v>
+      </c>
+      <c r="D59" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F59" s="98">
+        <f>B59+C59</f>
+        <v>6</v>
+      </c>
+      <c r="G59" s="99"/>
+      <c r="H59" s="129" t="s">
+        <v>203</v>
+      </c>
+      <c r="I59" s="128" t="s">
+        <v>202</v>
+      </c>
+      <c r="J59" s="126"/>
+    </row>
+    <row r="60" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="122" t="s">
+        <v>148</v>
+      </c>
+      <c r="B60" s="104">
+        <v>0</v>
+      </c>
+      <c r="C60" s="105">
+        <v>0</v>
+      </c>
+      <c r="D60" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E60" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="F60" s="111">
+        <f>B60+C60</f>
+        <v>0</v>
+      </c>
+      <c r="G60" s="99"/>
+      <c r="H60" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="I60" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J60" s="126"/>
+    </row>
+    <row r="61" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="119" t="s">
+        <v>149</v>
+      </c>
+      <c r="B61" s="112">
+        <v>79</v>
+      </c>
+      <c r="C61" s="112"/>
+      <c r="D61" s="112"/>
+      <c r="E61" s="112"/>
+      <c r="F61" s="113"/>
+      <c r="G61" s="102"/>
+      <c r="H61" s="130"/>
+      <c r="I61" s="130"/>
+      <c r="J61" s="130"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A62" s="133" t="s">
+        <v>220</v>
+      </c>
+      <c r="G62" s="102"/>
+    </row>
+    <row r="63" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G63" s="102"/>
+    </row>
+    <row r="64" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="119" t="s">
+        <v>156</v>
+      </c>
+      <c r="B64" s="115" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="D64" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="E64" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="F64" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="G64" s="110"/>
+      <c r="H64" s="123" t="s">
+        <v>140</v>
+      </c>
+      <c r="I64" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="J64" s="125" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" s="120" t="s">
+        <v>144</v>
+      </c>
+      <c r="B65" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="106">
+        <v>1</v>
+      </c>
+      <c r="D65" s="106">
+        <v>2</v>
+      </c>
+      <c r="E65" s="106" t="s">
+        <v>161</v>
+      </c>
+      <c r="F65" s="107">
+        <f>C65+D65</f>
+        <v>3</v>
+      </c>
+      <c r="G65" s="99"/>
+      <c r="H65" s="126"/>
+      <c r="I65" s="127" t="s">
+        <v>204</v>
+      </c>
+      <c r="J65" s="127" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A66" s="121" t="s">
+        <v>145</v>
+      </c>
+      <c r="B66" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C66" s="97">
+        <v>1</v>
+      </c>
+      <c r="D66" s="97">
+        <v>1</v>
+      </c>
+      <c r="E66" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F66" s="98">
+        <f t="shared" ref="F66:F67" si="7">C66+D66</f>
+        <v>2</v>
+      </c>
+      <c r="G66" s="99"/>
+      <c r="H66" s="126"/>
+      <c r="I66" s="128" t="s">
+        <v>205</v>
+      </c>
+      <c r="J66" s="128" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A67" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="B67" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C67" s="97">
+        <v>1</v>
+      </c>
+      <c r="D67" s="97">
+        <v>1</v>
+      </c>
+      <c r="E67" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F67" s="98">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="G67" s="99"/>
+      <c r="H67" s="126"/>
+      <c r="I67" s="128" t="s">
+        <v>206</v>
+      </c>
+      <c r="J67" s="128" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="121" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68" s="100">
+        <v>3</v>
+      </c>
+      <c r="C68" s="97">
+        <v>2</v>
+      </c>
+      <c r="D68" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E68" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F68" s="98">
+        <f>B68+C68</f>
+        <v>5</v>
+      </c>
+      <c r="G68" s="99"/>
+      <c r="H68" s="129" t="s">
+        <v>208</v>
+      </c>
+      <c r="I68" s="128" t="s">
+        <v>209</v>
+      </c>
+      <c r="J68" s="126"/>
+    </row>
+    <row r="69" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="122" t="s">
+        <v>148</v>
+      </c>
+      <c r="B69" s="104">
+        <v>0</v>
+      </c>
+      <c r="C69" s="105">
+        <v>0</v>
+      </c>
+      <c r="D69" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E69" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="F69" s="111">
+        <f>B69+C69</f>
+        <v>0</v>
+      </c>
+      <c r="G69" s="99"/>
+      <c r="H69" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="I69" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J69" s="126"/>
+    </row>
+    <row r="70" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="119" t="s">
+        <v>149</v>
+      </c>
+      <c r="B70" s="112">
+        <v>58</v>
+      </c>
+      <c r="C70" s="112"/>
+      <c r="D70" s="112"/>
+      <c r="E70" s="112"/>
+      <c r="F70" s="113"/>
+      <c r="G70" s="102"/>
+      <c r="H70" s="130"/>
+      <c r="I70" s="130"/>
+      <c r="J70" s="130"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A71" s="133" t="s">
+        <v>221</v>
+      </c>
+      <c r="G71" s="102"/>
+    </row>
+    <row r="72" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G72" s="102"/>
+    </row>
+    <row r="73" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="119" t="s">
+        <v>157</v>
+      </c>
+      <c r="B73" s="115" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="D73" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="E73" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="F73" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="G73" s="110"/>
+      <c r="H73" s="123" t="s">
+        <v>140</v>
+      </c>
+      <c r="I73" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="J73" s="125" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A74" s="120" t="s">
+        <v>144</v>
+      </c>
+      <c r="B74" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C74" s="106">
+        <v>1</v>
+      </c>
+      <c r="D74" s="106">
+        <v>1</v>
+      </c>
+      <c r="E74" s="106" t="s">
+        <v>161</v>
+      </c>
+      <c r="F74" s="107">
+        <f>C74+D74</f>
+        <v>2</v>
+      </c>
+      <c r="G74" s="99"/>
+      <c r="H74" s="126"/>
+      <c r="I74" s="127" t="s">
+        <v>210</v>
+      </c>
+      <c r="J74" s="127" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A75" s="121" t="s">
+        <v>145</v>
+      </c>
+      <c r="B75" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C75" s="97">
+        <v>2</v>
+      </c>
+      <c r="D75" s="97">
+        <v>1</v>
+      </c>
+      <c r="E75" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F75" s="98">
+        <f t="shared" ref="F75:F76" si="8">C75+D75</f>
+        <v>3</v>
+      </c>
+      <c r="G75" s="99"/>
+      <c r="H75" s="126"/>
+      <c r="I75" s="128" t="s">
+        <v>211</v>
+      </c>
+      <c r="J75" s="128" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A76" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="B76" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C76" s="97">
+        <v>1</v>
+      </c>
+      <c r="D76" s="97">
+        <v>1</v>
+      </c>
+      <c r="E76" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F76" s="98">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="G76" s="99"/>
+      <c r="H76" s="126"/>
+      <c r="I76" s="128" t="s">
+        <v>206</v>
+      </c>
+      <c r="J76" s="128" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="121" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" s="100">
+        <v>3</v>
+      </c>
+      <c r="C77" s="97">
+        <v>3</v>
+      </c>
+      <c r="D77" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E77" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F77" s="98">
+        <f>B77+C77</f>
+        <v>6</v>
+      </c>
+      <c r="G77" s="99"/>
+      <c r="H77" s="129" t="s">
+        <v>213</v>
+      </c>
+      <c r="I77" s="128" t="s">
+        <v>212</v>
+      </c>
+      <c r="J77" s="126"/>
+    </row>
+    <row r="78" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="122" t="s">
+        <v>148</v>
+      </c>
+      <c r="B78" s="104">
+        <v>0</v>
+      </c>
+      <c r="C78" s="105">
+        <v>0</v>
+      </c>
+      <c r="D78" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E78" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="F78" s="111">
+        <f>B78+C78</f>
+        <v>0</v>
+      </c>
+      <c r="G78" s="99"/>
+      <c r="H78" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="I78" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J78" s="126"/>
+    </row>
+    <row r="79" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="119" t="s">
+        <v>149</v>
+      </c>
+      <c r="B79" s="112">
+        <v>66</v>
+      </c>
+      <c r="C79" s="112"/>
+      <c r="D79" s="112"/>
+      <c r="E79" s="112"/>
+      <c r="F79" s="113"/>
+      <c r="G79" s="102"/>
+      <c r="H79" s="130"/>
+      <c r="I79" s="130"/>
+      <c r="J79" s="130"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A80" s="133" t="s">
+        <v>222</v>
+      </c>
+      <c r="G80" s="102"/>
+    </row>
+    <row r="81" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G81" s="102"/>
+    </row>
+    <row r="82" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="119" t="s">
+        <v>158</v>
+      </c>
+      <c r="B82" s="115" t="s">
+        <v>135</v>
+      </c>
+      <c r="C82" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="D82" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="E82" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="F82" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="G82" s="110"/>
+      <c r="H82" s="123" t="s">
+        <v>140</v>
+      </c>
+      <c r="I82" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="J82" s="125" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A83" s="120" t="s">
+        <v>144</v>
+      </c>
+      <c r="B83" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C83" s="106">
+        <v>3</v>
+      </c>
+      <c r="D83" s="106">
+        <v>1</v>
+      </c>
+      <c r="E83" s="106" t="s">
+        <v>161</v>
+      </c>
+      <c r="F83" s="107">
+        <f>C83+D83</f>
+        <v>4</v>
+      </c>
+      <c r="G83" s="99"/>
+      <c r="H83" s="126"/>
+      <c r="I83" s="127" t="s">
+        <v>214</v>
+      </c>
+      <c r="J83" s="127" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" s="121" t="s">
+        <v>145</v>
+      </c>
+      <c r="B84" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C84" s="97">
+        <v>3</v>
+      </c>
+      <c r="D84" s="97">
+        <v>1</v>
+      </c>
+      <c r="E84" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F84" s="98">
+        <f t="shared" ref="F84:F85" si="9">C84+D84</f>
+        <v>4</v>
+      </c>
+      <c r="G84" s="99"/>
+      <c r="H84" s="126"/>
+      <c r="I84" s="128" t="s">
+        <v>215</v>
+      </c>
+      <c r="J84" s="128" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A85" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="B85" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C85" s="97">
+        <v>1</v>
+      </c>
+      <c r="D85" s="97">
+        <v>1</v>
+      </c>
+      <c r="E85" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F85" s="98">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="G85" s="99"/>
+      <c r="H85" s="126"/>
+      <c r="I85" s="128" t="s">
+        <v>216</v>
+      </c>
+      <c r="J85" s="128" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A86" s="121" t="s">
+        <v>147</v>
+      </c>
+      <c r="B86" s="100">
+        <v>3</v>
+      </c>
+      <c r="C86" s="97">
+        <v>3</v>
+      </c>
+      <c r="D86" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E86" s="97" t="s">
+        <v>161</v>
+      </c>
+      <c r="F86" s="98">
+        <f>B86+C86</f>
+        <v>6</v>
+      </c>
+      <c r="G86" s="99"/>
+      <c r="H86" s="129" t="s">
+        <v>217</v>
+      </c>
+      <c r="I86" s="128" t="s">
+        <v>218</v>
+      </c>
+      <c r="J86" s="126"/>
+    </row>
+    <row r="87" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="122" t="s">
+        <v>148</v>
+      </c>
+      <c r="B87" s="104">
+        <v>0</v>
+      </c>
+      <c r="C87" s="105">
+        <v>0</v>
+      </c>
+      <c r="D87" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E87" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="F87" s="111">
+        <f>B87+C87</f>
+        <v>0</v>
+      </c>
+      <c r="G87" s="99"/>
+      <c r="H87" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="I87" s="132" t="s">
+        <v>128</v>
+      </c>
+      <c r="J87" s="126"/>
+    </row>
+    <row r="88" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="119" t="s">
+        <v>149</v>
+      </c>
+      <c r="B88" s="112">
+        <v>76</v>
+      </c>
+      <c r="C88" s="112"/>
+      <c r="D88" s="112"/>
+      <c r="E88" s="112"/>
+      <c r="F88" s="113"/>
+      <c r="G88" s="102"/>
+      <c r="H88" s="130"/>
+      <c r="I88" s="130"/>
+      <c r="J88" s="130"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A89" s="133" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B52:F52"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E11:E15 E20:E24 E29:E33 E38:E42 E47:E51 E56:E60 E65:E69 E74:E78 E83:E87" xr:uid="{CD716219-8A48-43EC-BAE4-39235EF81735}">
+      <formula1>$O$2:$Q$2</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="O1" r:id="rId1" location="FPCalc" display="http://groups.umd.umich.edu/cis/course.des/cis525/js/f00/harvey/FP_Calc.html?tCountVal=0 - FPCalc" xr:uid="{178087EB-D663-4E17-A671-DDD1ED445624}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[DHTD-107] update of time sheet up to now
</commit_message>
<xml_diff>
--- a/midterm-presentation/TimeSheet.xlsx
+++ b/midterm-presentation/TimeSheet.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programmierung\Android\Tower-Defense\midterm-presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA378C5-34A3-46C0-ACD9-6FCE92936472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B10EBF-C9AB-411A-9DA3-98FE0FE7CD38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TicketLog3rdS" sheetId="1" r:id="rId1"/>
     <sheet name="Charts3rdS" sheetId="2" r:id="rId2"/>
-    <sheet name="Use Case Overview" sheetId="3" r:id="rId3"/>
-    <sheet name="FP Calculation" sheetId="4" r:id="rId4"/>
+    <sheet name="TicketLog4thS" sheetId="5" r:id="rId3"/>
+    <sheet name="Use Case Overview" sheetId="3" r:id="rId4"/>
+    <sheet name="FP Calculation" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="331">
   <si>
     <t>Ticketart</t>
   </si>
@@ -706,6 +707,327 @@
   </si>
   <si>
     <t>Estimation: 9,1h</t>
+  </si>
+  <si>
+    <t>DHTD-55</t>
+  </si>
+  <si>
+    <t>Create UCS for UC "Upgrade Towers"</t>
+  </si>
+  <si>
+    <t>upgrade towers</t>
+  </si>
+  <si>
+    <t>DHTD-56</t>
+  </si>
+  <si>
+    <t>Create UCS for UC "Sell Towers"</t>
+  </si>
+  <si>
+    <t>sell towers</t>
+  </si>
+  <si>
+    <t>DHTD-57</t>
+  </si>
+  <si>
+    <t>Create UCS for UC "Select between different Towers"</t>
+  </si>
+  <si>
+    <t>select beween different towers</t>
+  </si>
+  <si>
+    <t>DHTD-58</t>
+  </si>
+  <si>
+    <t>edit settings</t>
+  </si>
+  <si>
+    <t>Create UCS for UC "Edit Settings"</t>
+  </si>
+  <si>
+    <t>DHTD-59</t>
+  </si>
+  <si>
+    <t>Create UCS for UC "Toggle Sound &amp; Animations"</t>
+  </si>
+  <si>
+    <t>toggle sound &amp; animations</t>
+  </si>
+  <si>
+    <t>DHTD-60</t>
+  </si>
+  <si>
+    <t>Create UCS for UC "Play multiple Levels with different Difficulties"</t>
+  </si>
+  <si>
+    <t>DHTD-61</t>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>Refactor Blog-Links</t>
+  </si>
+  <si>
+    <t>DHTD-62</t>
+  </si>
+  <si>
+    <t>Refactor Activity Diagrams of first 4 Use Cases</t>
+  </si>
+  <si>
+    <t>DHTD-63</t>
+  </si>
+  <si>
+    <t>Check for the film of the .feature-file tests</t>
+  </si>
+  <si>
+    <t>DHTD-64</t>
+  </si>
+  <si>
+    <t>Generate Jira-Gantt-Chart and Pie-Chart (Workflow) [and Cumulative Chart]</t>
+  </si>
+  <si>
+    <t>DHTD-65</t>
+  </si>
+  <si>
+    <t>Refactor Jira-Sprint-Names (week X + one-word-description)</t>
+  </si>
+  <si>
+    <t>DHTD-66</t>
+  </si>
+  <si>
+    <t>Blog Entry Week 11</t>
+  </si>
+  <si>
+    <t>DHTD-67</t>
+  </si>
+  <si>
+    <t>Create Risk-Management Table and publish</t>
+  </si>
+  <si>
+    <t>DHTD-68</t>
+  </si>
+  <si>
+    <t>Create UC-Overview-Table</t>
+  </si>
+  <si>
+    <t>DHTD-69</t>
+  </si>
+  <si>
+    <t>Blog Entry Week 12</t>
+  </si>
+  <si>
+    <t>DHTD-70</t>
+  </si>
+  <si>
+    <t>Write comments to other groups (Week 12)</t>
+  </si>
+  <si>
+    <t>DHTD-71</t>
+  </si>
+  <si>
+    <t>Introduce soundtrack-theme on main page</t>
+  </si>
+  <si>
+    <t>DHTD-26</t>
+  </si>
+  <si>
+    <t>GE: imlement money</t>
+  </si>
+  <si>
+    <t>DHTD-27</t>
+  </si>
+  <si>
+    <t>GE: implement life points for the game</t>
+  </si>
+  <si>
+    <t>DHTD-72</t>
+  </si>
+  <si>
+    <t>Implement the menu for choosing different towers</t>
+  </si>
+  <si>
+    <t>select between different towers</t>
+  </si>
+  <si>
+    <t>DHTD-73</t>
+  </si>
+  <si>
+    <t>Implement UC "Choose Difficulties"</t>
+  </si>
+  <si>
+    <t>choose difficulties</t>
+  </si>
+  <si>
+    <t>DHTD-74</t>
+  </si>
+  <si>
+    <t>Write comments to other groups (Week 13)</t>
+  </si>
+  <si>
+    <t>DHTD-75</t>
+  </si>
+  <si>
+    <t>Blog Entry Week 13</t>
+  </si>
+  <si>
+    <t>DHTD-76</t>
+  </si>
+  <si>
+    <t>Refactoring of Risk Management and UC Table</t>
+  </si>
+  <si>
+    <t>DHTD-77</t>
+  </si>
+  <si>
+    <t>Function Points Calculation</t>
+  </si>
+  <si>
+    <t>DHTD-24</t>
+  </si>
+  <si>
+    <t>Gameengine improve unit tests</t>
+  </si>
+  <si>
+    <t>DHTD-37</t>
+  </si>
+  <si>
+    <t>GE improve Bullet mechanism -&gt; avoid game crash and adjust calculations</t>
+  </si>
+  <si>
+    <t>DHTD-78</t>
+  </si>
+  <si>
+    <t>Implement UC Edit Settings</t>
+  </si>
+  <si>
+    <t>DHTD-79</t>
+  </si>
+  <si>
+    <t>Implement UC upgrade and sell Tower</t>
+  </si>
+  <si>
+    <t>DHTD-80</t>
+  </si>
+  <si>
+    <t>Implement a new tower called freezer</t>
+  </si>
+  <si>
+    <t>DHTD-81</t>
+  </si>
+  <si>
+    <t>Implement new tower boombastic</t>
+  </si>
+  <si>
+    <t>DHTD-86</t>
+  </si>
+  <si>
+    <t>Blog Entry Week 14</t>
+  </si>
+  <si>
+    <t>DHTD-87</t>
+  </si>
+  <si>
+    <t>Write comments to other groups (Week 14)</t>
+  </si>
+  <si>
+    <t>DHTD-92</t>
+  </si>
+  <si>
+    <t>Implement explosion animation if enemy dies</t>
+  </si>
+  <si>
+    <t>DHTD-93</t>
+  </si>
+  <si>
+    <t>Create new design for tower freezer</t>
+  </si>
+  <si>
+    <t>DHTD-94</t>
+  </si>
+  <si>
+    <t>Setup Test Environment</t>
+  </si>
+  <si>
+    <t>DHTD-95</t>
+  </si>
+  <si>
+    <t>Create new design for tower boombastic</t>
+  </si>
+  <si>
+    <t>DHTD-45</t>
+  </si>
+  <si>
+    <t>create bullet-design and implement into the game</t>
+  </si>
+  <si>
+    <t>DHTD-82</t>
+  </si>
+  <si>
+    <t>Implement new plasmatower</t>
+  </si>
+  <si>
+    <t>DHTD-96</t>
+  </si>
+  <si>
+    <t>Blog Entry Week 15</t>
+  </si>
+  <si>
+    <t>DHTD-97</t>
+  </si>
+  <si>
+    <t>Write comments to other groups (Week 15)</t>
+  </si>
+  <si>
+    <t>DHTD-98</t>
+  </si>
+  <si>
+    <t>Refactoring of given project</t>
+  </si>
+  <si>
+    <t>DHTD-99</t>
+  </si>
+  <si>
+    <t>Create design for tower plasmarizer</t>
+  </si>
+  <si>
+    <t>DHTD-100</t>
+  </si>
+  <si>
+    <t>Create design for tower assault laser</t>
+  </si>
+  <si>
+    <t>DHTD-83</t>
+  </si>
+  <si>
+    <t>Implement new laser tower</t>
+  </si>
+  <si>
+    <t>DHTD-101</t>
+  </si>
+  <si>
+    <t>Blog Entry Week 16</t>
+  </si>
+  <si>
+    <t>DHTD-102</t>
+  </si>
+  <si>
+    <t>Write comments to other groups (Week 16)</t>
+  </si>
+  <si>
+    <t>DHTD-103</t>
+  </si>
+  <si>
+    <t>Create designs/icons for settings menu</t>
+  </si>
+  <si>
+    <t>DHTD-105</t>
+  </si>
+  <si>
+    <t>Add design pattern to project</t>
+  </si>
+  <si>
+    <t>Project Management (h)</t>
   </si>
 </sst>
 </file>
@@ -802,7 +1124,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -1310,13 +1632,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1517,12 +1878,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1573,6 +1928,21 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Akzent3" xfId="1" builtinId="37"/>
@@ -7233,9 +7603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -9241,12 +9609,2100 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50C860A-1B08-4855-95EB-100DD969983E}">
+  <dimension ref="A1:Q93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.7265625" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="39.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.08984375" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1"/>
+    <col min="9" max="9" width="20.81640625" customWidth="1"/>
+    <col min="12" max="17" width="17.81640625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="77" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="134" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="135" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="135" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="136" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" s="135" t="s">
+        <v>226</v>
+      </c>
+      <c r="F2" s="135">
+        <v>2</v>
+      </c>
+      <c r="G2" s="135">
+        <v>3.75</v>
+      </c>
+      <c r="H2" s="135" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="137">
+        <v>0.5</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="5">
+        <f>SUM(N2:Q2)</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="138"/>
+      <c r="B3" s="138"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="138">
+        <v>2.5</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="3">
+        <f>SUM(N3:Q3)</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="3">
+        <f>SUM(N4:Q4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="5">
+        <f>SUM(N2:N4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="3">
+        <f>SUM(O2:O4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12" s="3">
+        <f>SUM(P2:P4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M13" s="3">
+        <f>SUM(Q2:Q4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="M17" s="5">
+        <f>SUM(G2,G55/2)</f>
+        <v>11.125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="M18" s="3">
+        <f>SUM(G5,G55/2)</f>
+        <v>10.125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="M19" s="3">
+        <f>SUM(G8,G35)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="M20" s="3">
+        <f>SUM(G9,G52)</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="M21" s="3">
+        <f>SUM(G10)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="M22" s="3">
+        <f>SUM(G13,G38)</f>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1">
+        <v>8</v>
+      </c>
+      <c r="G33" s="1">
+        <v>8</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I33" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1">
+        <v>4</v>
+      </c>
+      <c r="G34" s="1">
+        <v>2</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F35" s="1">
+        <v>16</v>
+      </c>
+      <c r="G35" s="1">
+        <v>24</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I36" s="1">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F38" s="1">
+        <v>10</v>
+      </c>
+      <c r="G38" s="1">
+        <v>13.25</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I40" s="1">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G42" s="1">
+        <v>2</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1">
+        <v>4</v>
+      </c>
+      <c r="G45" s="1">
+        <v>6</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I45" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I46" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1">
+        <v>6</v>
+      </c>
+      <c r="G48" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1">
+        <v>5</v>
+      </c>
+      <c r="G49" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" s="1">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F52" s="1">
+        <v>8</v>
+      </c>
+      <c r="G52" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I52" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F55" s="1">
+        <v>12</v>
+      </c>
+      <c r="G55" s="1">
+        <v>14.75</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I55" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56" s="1">
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1">
+        <v>8</v>
+      </c>
+      <c r="G58" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I58" s="1">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I59" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1">
+        <v>8</v>
+      </c>
+      <c r="G61" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I61" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1">
+        <v>3</v>
+      </c>
+      <c r="G64" s="1">
+        <v>2</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I65" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G66" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I66" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1">
+        <v>2</v>
+      </c>
+      <c r="G67" s="1">
+        <v>2</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I67" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1">
+        <v>3</v>
+      </c>
+      <c r="G68" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I68" s="1">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1">
+        <v>8</v>
+      </c>
+      <c r="G69" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I69" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1">
+        <v>3</v>
+      </c>
+      <c r="G70" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I70" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1">
+        <v>1</v>
+      </c>
+      <c r="G71" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I71" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1">
+        <v>5</v>
+      </c>
+      <c r="G72" s="1">
+        <v>8</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I72" s="1">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I73" s="1">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1">
+        <v>2</v>
+      </c>
+      <c r="G74" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I74" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I75" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I76" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1">
+        <v>1</v>
+      </c>
+      <c r="G77" s="1">
+        <v>1</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1">
+        <v>6</v>
+      </c>
+      <c r="G78" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I78" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I79" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I80" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1">
+        <v>3</v>
+      </c>
+      <c r="G81" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I81" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1">
+        <v>3</v>
+      </c>
+      <c r="G82" s="1">
+        <v>3</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I82" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1">
+        <v>12</v>
+      </c>
+      <c r="G83" s="1">
+        <v>14</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I83" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H84" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I84" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H85" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I85" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F86" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G86" s="1">
+        <v>2</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I86" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H87" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I87" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H88" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I88" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>324</v>
+      </c>
+      <c r="B89" t="s">
+        <v>242</v>
+      </c>
+      <c r="C89" t="s">
+        <v>57</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I89" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>326</v>
+      </c>
+      <c r="B90" t="s">
+        <v>18</v>
+      </c>
+      <c r="C90" t="s">
+        <v>57</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F90">
+        <v>1.5</v>
+      </c>
+      <c r="G90">
+        <v>2</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I90" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H91" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I91" s="1">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>328</v>
+      </c>
+      <c r="B92" t="s">
+        <v>18</v>
+      </c>
+      <c r="C92" t="s">
+        <v>57</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F92">
+        <v>8</v>
+      </c>
+      <c r="G92">
+        <v>3</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I92" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H93" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I93" s="1">
+        <v>2.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C55BAC4-B6C8-4445-BEEB-A5DE06A20711}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -9492,25 +11948,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3800D6FA-69EA-4E12-9E16-1909B3CAE7B3}">
   <dimension ref="A1:Q89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37.1796875" style="94" customWidth="1"/>
     <col min="2" max="7" width="10.90625" style="101"/>
-    <col min="8" max="9" width="19.6328125" style="131" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" style="131" customWidth="1"/>
+    <col min="8" max="9" width="19.6328125" style="129" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" style="129" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="91" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="117" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="113" t="s">
         <v>135</v>
       </c>
       <c r="C1" s="108" t="s">
@@ -9526,13 +11982,13 @@
         <v>139</v>
       </c>
       <c r="G1" s="110"/>
-      <c r="H1" s="123" t="s">
+      <c r="H1" s="121" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="124" t="s">
+      <c r="I1" s="122" t="s">
         <v>141</v>
       </c>
-      <c r="J1" s="125" t="s">
+      <c r="J1" s="123" t="s">
         <v>142</v>
       </c>
       <c r="M1" s="91" t="s">
@@ -9543,10 +11999,10 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="114" t="s">
         <v>128</v>
       </c>
       <c r="C2" s="106">
@@ -9563,11 +12019,11 @@
         <v>3</v>
       </c>
       <c r="G2" s="99"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="127" t="s">
+      <c r="H2" s="124"/>
+      <c r="I2" s="125" t="s">
         <v>182</v>
       </c>
-      <c r="J2" s="127" t="s">
+      <c r="J2" s="125" t="s">
         <v>170</v>
       </c>
       <c r="M2" s="91" t="s">
@@ -9584,10 +12040,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="119" t="s">
         <v>145</v>
       </c>
-      <c r="B3" s="117" t="s">
+      <c r="B3" s="115" t="s">
         <v>128</v>
       </c>
       <c r="C3" s="97">
@@ -9604,19 +12060,19 @@
         <v>6</v>
       </c>
       <c r="G3" s="99"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="128" t="s">
+      <c r="H3" s="124"/>
+      <c r="I3" s="126" t="s">
         <v>169</v>
       </c>
-      <c r="J3" s="128" t="s">
+      <c r="J3" s="126" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C4" s="97">
@@ -9633,11 +12089,11 @@
         <v>0</v>
       </c>
       <c r="G4" s="99"/>
-      <c r="H4" s="126"/>
-      <c r="I4" s="132" t="s">
+      <c r="H4" s="124"/>
+      <c r="I4" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J4" s="132" t="s">
+      <c r="J4" s="130" t="s">
         <v>128</v>
       </c>
       <c r="M4" t="s">
@@ -9645,7 +12101,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="119" t="s">
         <v>147</v>
       </c>
       <c r="B5" s="100">
@@ -9654,7 +12110,7 @@
       <c r="C5" s="97">
         <v>5</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E5" s="97" t="s">
@@ -9665,19 +12121,19 @@
         <v>7</v>
       </c>
       <c r="G5" s="99"/>
-      <c r="H5" s="129" t="s">
+      <c r="H5" s="127" t="s">
         <v>171</v>
       </c>
-      <c r="I5" s="128" t="s">
+      <c r="I5" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="J5" s="126"/>
+      <c r="J5" s="124"/>
       <c r="M5" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="120" t="s">
         <v>148</v>
       </c>
       <c r="B6" s="104">
@@ -9686,7 +12142,7 @@
       <c r="C6" s="105">
         <v>0</v>
       </c>
-      <c r="D6" s="114" t="s">
+      <c r="D6" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E6" s="105" t="s">
@@ -9697,39 +12153,39 @@
         <v>0</v>
       </c>
       <c r="G6" s="99"/>
-      <c r="H6" s="132" t="s">
+      <c r="H6" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="I6" s="132" t="s">
+      <c r="I6" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J6" s="126"/>
+      <c r="J6" s="124"/>
       <c r="M6" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="119" t="s">
+      <c r="A7" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="112">
+      <c r="B7" s="132">
         <v>82</v>
       </c>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="113"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="133"/>
       <c r="G7" s="102"/>
-      <c r="H7" s="130"/>
-      <c r="I7" s="130"/>
-      <c r="J7" s="130"/>
+      <c r="H7" s="128"/>
+      <c r="I7" s="128"/>
+      <c r="J7" s="128"/>
     </row>
     <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="119" t="s">
+      <c r="A10" s="117" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="115" t="s">
+      <c r="B10" s="113" t="s">
         <v>135</v>
       </c>
       <c r="C10" s="108" t="s">
@@ -9745,21 +12201,21 @@
         <v>139</v>
       </c>
       <c r="G10" s="110"/>
-      <c r="H10" s="123" t="s">
+      <c r="H10" s="121" t="s">
         <v>140</v>
       </c>
-      <c r="I10" s="124" t="s">
+      <c r="I10" s="122" t="s">
         <v>141</v>
       </c>
-      <c r="J10" s="125" t="s">
+      <c r="J10" s="123" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="120" t="s">
+      <c r="A11" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C11" s="106">
@@ -9776,19 +12232,19 @@
         <v>3</v>
       </c>
       <c r="G11" s="99"/>
-      <c r="H11" s="126"/>
-      <c r="I11" s="127" t="s">
+      <c r="H11" s="124"/>
+      <c r="I11" s="125" t="s">
         <v>173</v>
       </c>
-      <c r="J11" s="127" t="s">
+      <c r="J11" s="125" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="119" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C12" s="97">
@@ -9805,19 +12261,19 @@
         <v>4</v>
       </c>
       <c r="G12" s="99"/>
-      <c r="H12" s="126"/>
-      <c r="I12" s="128" t="s">
+      <c r="H12" s="124"/>
+      <c r="I12" s="126" t="s">
         <v>175</v>
       </c>
-      <c r="J12" s="128" t="s">
+      <c r="J12" s="126" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="121" t="s">
+      <c r="A13" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C13" s="97">
@@ -9834,16 +12290,16 @@
         <v>0</v>
       </c>
       <c r="G13" s="99"/>
-      <c r="H13" s="126"/>
-      <c r="I13" s="132" t="s">
+      <c r="H13" s="124"/>
+      <c r="I13" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="132" t="s">
+      <c r="J13" s="130" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="119" t="s">
         <v>147</v>
       </c>
       <c r="B14" s="100">
@@ -9852,7 +12308,7 @@
       <c r="C14" s="97">
         <v>5</v>
       </c>
-      <c r="D14" s="114" t="s">
+      <c r="D14" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E14" s="97" t="s">
@@ -9863,16 +12319,16 @@
         <v>8</v>
       </c>
       <c r="G14" s="99"/>
-      <c r="H14" s="129" t="s">
+      <c r="H14" s="127" t="s">
         <v>184</v>
       </c>
-      <c r="I14" s="128" t="s">
+      <c r="I14" s="126" t="s">
         <v>185</v>
       </c>
-      <c r="J14" s="126"/>
+      <c r="J14" s="124"/>
     </row>
     <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="122" t="s">
+      <c r="A15" s="120" t="s">
         <v>148</v>
       </c>
       <c r="B15" s="104">
@@ -9881,7 +12337,7 @@
       <c r="C15" s="105">
         <v>0</v>
       </c>
-      <c r="D15" s="114" t="s">
+      <c r="D15" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E15" s="105" t="s">
@@ -9892,36 +12348,36 @@
         <v>0</v>
       </c>
       <c r="G15" s="99"/>
-      <c r="H15" s="132" t="s">
+      <c r="H15" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="I15" s="132" t="s">
+      <c r="I15" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J15" s="126"/>
+      <c r="J15" s="124"/>
     </row>
     <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="119" t="s">
+      <c r="A16" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B16" s="112">
+      <c r="B16" s="132">
         <v>81</v>
       </c>
-      <c r="C16" s="112"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="112"/>
-      <c r="F16" s="113"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="132"/>
+      <c r="F16" s="133"/>
       <c r="G16" s="102"/>
-      <c r="H16" s="130"/>
-      <c r="I16" s="130"/>
-      <c r="J16" s="130"/>
+      <c r="H16" s="128"/>
+      <c r="I16" s="128"/>
+      <c r="J16" s="128"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="119" t="s">
+      <c r="A19" s="117" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="113" t="s">
         <v>135</v>
       </c>
       <c r="C19" s="108" t="s">
@@ -9937,21 +12393,21 @@
         <v>139</v>
       </c>
       <c r="G19" s="110"/>
-      <c r="H19" s="123" t="s">
+      <c r="H19" s="121" t="s">
         <v>140</v>
       </c>
-      <c r="I19" s="124" t="s">
+      <c r="I19" s="122" t="s">
         <v>141</v>
       </c>
-      <c r="J19" s="125" t="s">
+      <c r="J19" s="123" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="120" t="s">
+      <c r="A20" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B20" s="118" t="s">
+      <c r="B20" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C20" s="106">
@@ -9968,19 +12424,19 @@
         <v>5</v>
       </c>
       <c r="G20" s="99"/>
-      <c r="H20" s="126"/>
-      <c r="I20" s="127" t="s">
+      <c r="H20" s="124"/>
+      <c r="I20" s="125" t="s">
         <v>179</v>
       </c>
-      <c r="J20" s="127" t="s">
+      <c r="J20" s="125" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="121" t="s">
+      <c r="A21" s="119" t="s">
         <v>145</v>
       </c>
-      <c r="B21" s="118" t="s">
+      <c r="B21" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C21" s="97">
@@ -9997,19 +12453,19 @@
         <v>4</v>
       </c>
       <c r="G21" s="99"/>
-      <c r="H21" s="126"/>
-      <c r="I21" s="128" t="s">
+      <c r="H21" s="124"/>
+      <c r="I21" s="126" t="s">
         <v>186</v>
       </c>
-      <c r="J21" s="128" t="s">
+      <c r="J21" s="126" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="121" t="s">
+      <c r="A22" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="B22" s="118" t="s">
+      <c r="B22" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C22" s="97">
@@ -10026,16 +12482,16 @@
         <v>0</v>
       </c>
       <c r="G22" s="99"/>
-      <c r="H22" s="126"/>
-      <c r="I22" s="132" t="s">
+      <c r="H22" s="124"/>
+      <c r="I22" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J22" s="132" t="s">
+      <c r="J22" s="130" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="121" t="s">
+      <c r="A23" s="119" t="s">
         <v>147</v>
       </c>
       <c r="B23" s="100">
@@ -10044,7 +12500,7 @@
       <c r="C23" s="97">
         <v>2</v>
       </c>
-      <c r="D23" s="114" t="s">
+      <c r="D23" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E23" s="97" t="s">
@@ -10055,16 +12511,16 @@
         <v>4</v>
       </c>
       <c r="G23" s="99"/>
-      <c r="H23" s="129" t="s">
+      <c r="H23" s="127" t="s">
         <v>177</v>
       </c>
-      <c r="I23" s="128" t="s">
+      <c r="I23" s="126" t="s">
         <v>177</v>
       </c>
-      <c r="J23" s="126"/>
+      <c r="J23" s="124"/>
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="122" t="s">
+      <c r="A24" s="120" t="s">
         <v>148</v>
       </c>
       <c r="B24" s="104">
@@ -10073,7 +12529,7 @@
       <c r="C24" s="105">
         <v>0</v>
       </c>
-      <c r="D24" s="114" t="s">
+      <c r="D24" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E24" s="105" t="s">
@@ -10084,36 +12540,36 @@
         <v>0</v>
       </c>
       <c r="G24" s="99"/>
-      <c r="H24" s="132" t="s">
+      <c r="H24" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="I24" s="132" t="s">
+      <c r="I24" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J24" s="126"/>
+      <c r="J24" s="124"/>
     </row>
     <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="119" t="s">
+      <c r="A25" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B25" s="112">
+      <c r="B25" s="132">
         <v>64</v>
       </c>
-      <c r="C25" s="112"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="112"/>
-      <c r="F25" s="113"/>
+      <c r="C25" s="132"/>
+      <c r="D25" s="132"/>
+      <c r="E25" s="132"/>
+      <c r="F25" s="133"/>
       <c r="G25" s="102"/>
-      <c r="H25" s="130"/>
-      <c r="I25" s="130"/>
-      <c r="J25" s="130"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="128"/>
+      <c r="J25" s="128"/>
     </row>
     <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="119" t="s">
+      <c r="A28" s="117" t="s">
         <v>152</v>
       </c>
-      <c r="B28" s="115" t="s">
+      <c r="B28" s="113" t="s">
         <v>135</v>
       </c>
       <c r="C28" s="108" t="s">
@@ -10129,21 +12585,21 @@
         <v>139</v>
       </c>
       <c r="G28" s="110"/>
-      <c r="H28" s="123" t="s">
+      <c r="H28" s="121" t="s">
         <v>140</v>
       </c>
-      <c r="I28" s="124" t="s">
+      <c r="I28" s="122" t="s">
         <v>141</v>
       </c>
-      <c r="J28" s="125" t="s">
+      <c r="J28" s="123" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="120" t="s">
+      <c r="A29" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B29" s="118" t="s">
+      <c r="B29" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C29" s="106">
@@ -10160,19 +12616,19 @@
         <v>4</v>
       </c>
       <c r="G29" s="99"/>
-      <c r="H29" s="126"/>
-      <c r="I29" s="127" t="s">
+      <c r="H29" s="124"/>
+      <c r="I29" s="125" t="s">
         <v>181</v>
       </c>
-      <c r="J29" s="127" t="s">
+      <c r="J29" s="125" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="121" t="s">
+      <c r="A30" s="119" t="s">
         <v>145</v>
       </c>
-      <c r="B30" s="118" t="s">
+      <c r="B30" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C30" s="97">
@@ -10189,19 +12645,19 @@
         <v>1</v>
       </c>
       <c r="G30" s="99"/>
-      <c r="H30" s="126"/>
-      <c r="I30" s="128" t="s">
+      <c r="H30" s="124"/>
+      <c r="I30" s="126" t="s">
         <v>170</v>
       </c>
-      <c r="J30" s="132" t="s">
+      <c r="J30" s="130" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" s="121" t="s">
+      <c r="A31" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="B31" s="118" t="s">
+      <c r="B31" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C31" s="97">
@@ -10218,16 +12674,16 @@
         <v>0</v>
       </c>
       <c r="G31" s="99"/>
-      <c r="H31" s="126"/>
-      <c r="I31" s="132" t="s">
+      <c r="H31" s="124"/>
+      <c r="I31" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J31" s="132" t="s">
+      <c r="J31" s="130" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="121" t="s">
+      <c r="A32" s="119" t="s">
         <v>147</v>
       </c>
       <c r="B32" s="100">
@@ -10236,7 +12692,7 @@
       <c r="C32" s="97">
         <v>2</v>
       </c>
-      <c r="D32" s="114" t="s">
+      <c r="D32" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E32" s="97" t="s">
@@ -10247,16 +12703,16 @@
         <v>4</v>
       </c>
       <c r="G32" s="99"/>
-      <c r="H32" s="129" t="s">
+      <c r="H32" s="127" t="s">
         <v>183</v>
       </c>
-      <c r="I32" s="128" t="s">
+      <c r="I32" s="126" t="s">
         <v>183</v>
       </c>
-      <c r="J32" s="126"/>
+      <c r="J32" s="124"/>
     </row>
     <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="122" t="s">
+      <c r="A33" s="120" t="s">
         <v>148</v>
       </c>
       <c r="B33" s="104">
@@ -10265,7 +12721,7 @@
       <c r="C33" s="105">
         <v>0</v>
       </c>
-      <c r="D33" s="114" t="s">
+      <c r="D33" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E33" s="105" t="s">
@@ -10276,29 +12732,29 @@
         <v>0</v>
       </c>
       <c r="G33" s="99"/>
-      <c r="H33" s="132" t="s">
+      <c r="H33" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="I33" s="132" t="s">
+      <c r="I33" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J33" s="126"/>
+      <c r="J33" s="124"/>
     </row>
     <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="119" t="s">
+      <c r="A34" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B34" s="112">
+      <c r="B34" s="132">
         <v>44</v>
       </c>
-      <c r="C34" s="112"/>
-      <c r="D34" s="112"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="113"/>
+      <c r="C34" s="132"/>
+      <c r="D34" s="132"/>
+      <c r="E34" s="132"/>
+      <c r="F34" s="133"/>
       <c r="G34" s="102"/>
-      <c r="H34" s="130"/>
-      <c r="I34" s="130"/>
-      <c r="J34" s="130"/>
+      <c r="H34" s="128"/>
+      <c r="I34" s="128"/>
+      <c r="J34" s="128"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G35" s="102"/>
@@ -10307,10 +12763,10 @@
       <c r="G36" s="102"/>
     </row>
     <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="119" t="s">
+      <c r="A37" s="117" t="s">
         <v>153</v>
       </c>
-      <c r="B37" s="115" t="s">
+      <c r="B37" s="113" t="s">
         <v>135</v>
       </c>
       <c r="C37" s="108" t="s">
@@ -10326,21 +12782,21 @@
         <v>139</v>
       </c>
       <c r="G37" s="110"/>
-      <c r="H37" s="123" t="s">
+      <c r="H37" s="121" t="s">
         <v>140</v>
       </c>
-      <c r="I37" s="124" t="s">
+      <c r="I37" s="122" t="s">
         <v>141</v>
       </c>
-      <c r="J37" s="125" t="s">
+      <c r="J37" s="123" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="120" t="s">
+      <c r="A38" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B38" s="118" t="s">
+      <c r="B38" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C38" s="106">
@@ -10357,19 +12813,19 @@
         <v>4</v>
       </c>
       <c r="G38" s="99"/>
-      <c r="H38" s="126"/>
-      <c r="I38" s="127" t="s">
+      <c r="H38" s="124"/>
+      <c r="I38" s="125" t="s">
         <v>188</v>
       </c>
-      <c r="J38" s="127" t="s">
+      <c r="J38" s="125" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="121" t="s">
+      <c r="A39" s="119" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="118" t="s">
+      <c r="B39" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C39" s="97">
@@ -10386,19 +12842,19 @@
         <v>5</v>
       </c>
       <c r="G39" s="99"/>
-      <c r="H39" s="126"/>
-      <c r="I39" s="128" t="s">
+      <c r="H39" s="124"/>
+      <c r="I39" s="126" t="s">
         <v>194</v>
       </c>
-      <c r="J39" s="128" t="s">
+      <c r="J39" s="126" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="121" t="s">
+      <c r="A40" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="B40" s="118" t="s">
+      <c r="B40" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C40" s="97">
@@ -10415,16 +12871,16 @@
         <v>2</v>
       </c>
       <c r="G40" s="99"/>
-      <c r="H40" s="126"/>
-      <c r="I40" s="128" t="s">
+      <c r="H40" s="124"/>
+      <c r="I40" s="126" t="s">
         <v>190</v>
       </c>
-      <c r="J40" s="128" t="s">
+      <c r="J40" s="126" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="121" t="s">
+      <c r="A41" s="119" t="s">
         <v>147</v>
       </c>
       <c r="B41" s="100">
@@ -10433,7 +12889,7 @@
       <c r="C41" s="97">
         <v>3</v>
       </c>
-      <c r="D41" s="114" t="s">
+      <c r="D41" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E41" s="97" t="s">
@@ -10444,16 +12900,16 @@
         <v>6</v>
       </c>
       <c r="G41" s="99"/>
-      <c r="H41" s="129" t="s">
+      <c r="H41" s="127" t="s">
         <v>197</v>
       </c>
-      <c r="I41" s="128" t="s">
+      <c r="I41" s="126" t="s">
         <v>192</v>
       </c>
-      <c r="J41" s="126"/>
+      <c r="J41" s="124"/>
     </row>
     <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="122" t="s">
+      <c r="A42" s="120" t="s">
         <v>148</v>
       </c>
       <c r="B42" s="104">
@@ -10462,7 +12918,7 @@
       <c r="C42" s="105">
         <v>0</v>
       </c>
-      <c r="D42" s="114" t="s">
+      <c r="D42" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E42" s="105" t="s">
@@ -10473,33 +12929,33 @@
         <v>0</v>
       </c>
       <c r="G42" s="99"/>
-      <c r="H42" s="132" t="s">
+      <c r="H42" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="I42" s="132" t="s">
+      <c r="I42" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J42" s="126"/>
+      <c r="J42" s="124"/>
       <c r="K42" s="96"/>
     </row>
     <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="119" t="s">
+      <c r="A43" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B43" s="112">
+      <c r="B43" s="132">
         <v>80</v>
       </c>
-      <c r="C43" s="112"/>
-      <c r="D43" s="112"/>
-      <c r="E43" s="112"/>
-      <c r="F43" s="113"/>
+      <c r="C43" s="132"/>
+      <c r="D43" s="132"/>
+      <c r="E43" s="132"/>
+      <c r="F43" s="133"/>
       <c r="G43" s="102"/>
-      <c r="H43" s="130"/>
-      <c r="I43" s="130"/>
-      <c r="J43" s="130"/>
+      <c r="H43" s="128"/>
+      <c r="I43" s="128"/>
+      <c r="J43" s="128"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="133" t="s">
+      <c r="A44" s="131" t="s">
         <v>219</v>
       </c>
       <c r="G44" s="102"/>
@@ -10508,10 +12964,10 @@
       <c r="G45" s="102"/>
     </row>
     <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="119" t="s">
+      <c r="A46" s="117" t="s">
         <v>154</v>
       </c>
-      <c r="B46" s="115" t="s">
+      <c r="B46" s="113" t="s">
         <v>135</v>
       </c>
       <c r="C46" s="108" t="s">
@@ -10527,21 +12983,21 @@
         <v>139</v>
       </c>
       <c r="G46" s="110"/>
-      <c r="H46" s="123" t="s">
+      <c r="H46" s="121" t="s">
         <v>140</v>
       </c>
-      <c r="I46" s="124" t="s">
+      <c r="I46" s="122" t="s">
         <v>141</v>
       </c>
-      <c r="J46" s="125" t="s">
+      <c r="J46" s="123" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="120" t="s">
+      <c r="A47" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B47" s="118" t="s">
+      <c r="B47" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C47" s="106">
@@ -10558,19 +13014,19 @@
         <v>4</v>
       </c>
       <c r="G47" s="99"/>
-      <c r="H47" s="126"/>
-      <c r="I47" s="127" t="s">
+      <c r="H47" s="124"/>
+      <c r="I47" s="125" t="s">
         <v>193</v>
       </c>
-      <c r="J47" s="127" t="s">
+      <c r="J47" s="125" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="121" t="s">
+      <c r="A48" s="119" t="s">
         <v>145</v>
       </c>
-      <c r="B48" s="118" t="s">
+      <c r="B48" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C48" s="97">
@@ -10587,19 +13043,19 @@
         <v>5</v>
       </c>
       <c r="G48" s="99"/>
-      <c r="H48" s="126"/>
-      <c r="I48" s="128" t="s">
+      <c r="H48" s="124"/>
+      <c r="I48" s="126" t="s">
         <v>194</v>
       </c>
-      <c r="J48" s="128" t="s">
+      <c r="J48" s="126" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A49" s="121" t="s">
+      <c r="A49" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="B49" s="118" t="s">
+      <c r="B49" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C49" s="97">
@@ -10616,16 +13072,16 @@
         <v>2</v>
       </c>
       <c r="G49" s="99"/>
-      <c r="H49" s="126"/>
-      <c r="I49" s="128" t="s">
+      <c r="H49" s="124"/>
+      <c r="I49" s="126" t="s">
         <v>190</v>
       </c>
-      <c r="J49" s="128" t="s">
+      <c r="J49" s="126" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A50" s="121" t="s">
+      <c r="A50" s="119" t="s">
         <v>147</v>
       </c>
       <c r="B50" s="100">
@@ -10634,7 +13090,7 @@
       <c r="C50" s="97">
         <v>3</v>
       </c>
-      <c r="D50" s="114" t="s">
+      <c r="D50" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E50" s="97" t="s">
@@ -10645,16 +13101,16 @@
         <v>6</v>
       </c>
       <c r="G50" s="99"/>
-      <c r="H50" s="129" t="s">
+      <c r="H50" s="127" t="s">
         <v>196</v>
       </c>
-      <c r="I50" s="128" t="s">
+      <c r="I50" s="126" t="s">
         <v>195</v>
       </c>
-      <c r="J50" s="126"/>
+      <c r="J50" s="124"/>
     </row>
     <row r="51" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="122" t="s">
+      <c r="A51" s="120" t="s">
         <v>148</v>
       </c>
       <c r="B51" s="104">
@@ -10663,7 +13119,7 @@
       <c r="C51" s="105">
         <v>0</v>
       </c>
-      <c r="D51" s="114" t="s">
+      <c r="D51" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E51" s="105" t="s">
@@ -10674,32 +13130,32 @@
         <v>0</v>
       </c>
       <c r="G51" s="99"/>
-      <c r="H51" s="132" t="s">
+      <c r="H51" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="I51" s="132" t="s">
+      <c r="I51" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J51" s="126"/>
+      <c r="J51" s="124"/>
     </row>
     <row r="52" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="119" t="s">
+      <c r="A52" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B52" s="112">
+      <c r="B52" s="132">
         <v>80</v>
       </c>
-      <c r="C52" s="112"/>
-      <c r="D52" s="112"/>
-      <c r="E52" s="112"/>
-      <c r="F52" s="113"/>
+      <c r="C52" s="132"/>
+      <c r="D52" s="132"/>
+      <c r="E52" s="132"/>
+      <c r="F52" s="133"/>
       <c r="G52" s="102"/>
-      <c r="H52" s="130"/>
-      <c r="I52" s="130"/>
-      <c r="J52" s="130"/>
+      <c r="H52" s="128"/>
+      <c r="I52" s="128"/>
+      <c r="J52" s="128"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A53" s="133" t="s">
+      <c r="A53" s="131" t="s">
         <v>219</v>
       </c>
       <c r="G53" s="102"/>
@@ -10708,10 +13164,10 @@
       <c r="G54" s="102"/>
     </row>
     <row r="55" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="119" t="s">
+      <c r="A55" s="117" t="s">
         <v>155</v>
       </c>
-      <c r="B55" s="115" t="s">
+      <c r="B55" s="113" t="s">
         <v>135</v>
       </c>
       <c r="C55" s="108" t="s">
@@ -10727,21 +13183,21 @@
         <v>139</v>
       </c>
       <c r="G55" s="110"/>
-      <c r="H55" s="123" t="s">
+      <c r="H55" s="121" t="s">
         <v>140</v>
       </c>
-      <c r="I55" s="124" t="s">
+      <c r="I55" s="122" t="s">
         <v>141</v>
       </c>
-      <c r="J55" s="125" t="s">
+      <c r="J55" s="123" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A56" s="120" t="s">
+      <c r="A56" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B56" s="118" t="s">
+      <c r="B56" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C56" s="106">
@@ -10758,19 +13214,19 @@
         <v>4</v>
       </c>
       <c r="G56" s="99"/>
-      <c r="H56" s="126"/>
-      <c r="I56" s="127" t="s">
+      <c r="H56" s="124"/>
+      <c r="I56" s="125" t="s">
         <v>198</v>
       </c>
-      <c r="J56" s="127" t="s">
+      <c r="J56" s="125" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="121" t="s">
+      <c r="A57" s="119" t="s">
         <v>145</v>
       </c>
-      <c r="B57" s="118" t="s">
+      <c r="B57" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C57" s="97">
@@ -10787,19 +13243,19 @@
         <v>4</v>
       </c>
       <c r="G57" s="99"/>
-      <c r="H57" s="126"/>
-      <c r="I57" s="128" t="s">
+      <c r="H57" s="124"/>
+      <c r="I57" s="126" t="s">
         <v>200</v>
       </c>
-      <c r="J57" s="128" t="s">
+      <c r="J57" s="126" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A58" s="121" t="s">
+      <c r="A58" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="B58" s="118" t="s">
+      <c r="B58" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C58" s="97">
@@ -10816,16 +13272,16 @@
         <v>3</v>
       </c>
       <c r="G58" s="99"/>
-      <c r="H58" s="126"/>
-      <c r="I58" s="128" t="s">
+      <c r="H58" s="124"/>
+      <c r="I58" s="126" t="s">
         <v>201</v>
       </c>
-      <c r="J58" s="128" t="s">
+      <c r="J58" s="126" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" s="121" t="s">
+      <c r="A59" s="119" t="s">
         <v>147</v>
       </c>
       <c r="B59" s="100">
@@ -10834,7 +13290,7 @@
       <c r="C59" s="97">
         <v>3</v>
       </c>
-      <c r="D59" s="114" t="s">
+      <c r="D59" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E59" s="97" t="s">
@@ -10845,16 +13301,16 @@
         <v>6</v>
       </c>
       <c r="G59" s="99"/>
-      <c r="H59" s="129" t="s">
+      <c r="H59" s="127" t="s">
         <v>203</v>
       </c>
-      <c r="I59" s="128" t="s">
+      <c r="I59" s="126" t="s">
         <v>202</v>
       </c>
-      <c r="J59" s="126"/>
+      <c r="J59" s="124"/>
     </row>
     <row r="60" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="122" t="s">
+      <c r="A60" s="120" t="s">
         <v>148</v>
       </c>
       <c r="B60" s="104">
@@ -10863,7 +13319,7 @@
       <c r="C60" s="105">
         <v>0</v>
       </c>
-      <c r="D60" s="114" t="s">
+      <c r="D60" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E60" s="105" t="s">
@@ -10874,32 +13330,32 @@
         <v>0</v>
       </c>
       <c r="G60" s="99"/>
-      <c r="H60" s="132" t="s">
+      <c r="H60" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="I60" s="132" t="s">
+      <c r="I60" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J60" s="126"/>
+      <c r="J60" s="124"/>
     </row>
     <row r="61" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="119" t="s">
+      <c r="A61" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B61" s="112">
+      <c r="B61" s="132">
         <v>79</v>
       </c>
-      <c r="C61" s="112"/>
-      <c r="D61" s="112"/>
-      <c r="E61" s="112"/>
-      <c r="F61" s="113"/>
+      <c r="C61" s="132"/>
+      <c r="D61" s="132"/>
+      <c r="E61" s="132"/>
+      <c r="F61" s="133"/>
       <c r="G61" s="102"/>
-      <c r="H61" s="130"/>
-      <c r="I61" s="130"/>
-      <c r="J61" s="130"/>
+      <c r="H61" s="128"/>
+      <c r="I61" s="128"/>
+      <c r="J61" s="128"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A62" s="133" t="s">
+      <c r="A62" s="131" t="s">
         <v>220</v>
       </c>
       <c r="G62" s="102"/>
@@ -10908,10 +13364,10 @@
       <c r="G63" s="102"/>
     </row>
     <row r="64" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="119" t="s">
+      <c r="A64" s="117" t="s">
         <v>156</v>
       </c>
-      <c r="B64" s="115" t="s">
+      <c r="B64" s="113" t="s">
         <v>135</v>
       </c>
       <c r="C64" s="108" t="s">
@@ -10927,21 +13383,21 @@
         <v>139</v>
       </c>
       <c r="G64" s="110"/>
-      <c r="H64" s="123" t="s">
+      <c r="H64" s="121" t="s">
         <v>140</v>
       </c>
-      <c r="I64" s="124" t="s">
+      <c r="I64" s="122" t="s">
         <v>141</v>
       </c>
-      <c r="J64" s="125" t="s">
+      <c r="J64" s="123" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="120" t="s">
+      <c r="A65" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B65" s="118" t="s">
+      <c r="B65" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C65" s="106">
@@ -10958,19 +13414,19 @@
         <v>3</v>
       </c>
       <c r="G65" s="99"/>
-      <c r="H65" s="126"/>
-      <c r="I65" s="127" t="s">
+      <c r="H65" s="124"/>
+      <c r="I65" s="125" t="s">
         <v>204</v>
       </c>
-      <c r="J65" s="127" t="s">
+      <c r="J65" s="125" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A66" s="121" t="s">
+      <c r="A66" s="119" t="s">
         <v>145</v>
       </c>
-      <c r="B66" s="118" t="s">
+      <c r="B66" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C66" s="97">
@@ -10987,19 +13443,19 @@
         <v>2</v>
       </c>
       <c r="G66" s="99"/>
-      <c r="H66" s="126"/>
-      <c r="I66" s="128" t="s">
+      <c r="H66" s="124"/>
+      <c r="I66" s="126" t="s">
         <v>205</v>
       </c>
-      <c r="J66" s="128" t="s">
+      <c r="J66" s="126" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="121" t="s">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A67" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="B67" s="118" t="s">
+      <c r="B67" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C67" s="97">
@@ -11016,16 +13472,16 @@
         <v>2</v>
       </c>
       <c r="G67" s="99"/>
-      <c r="H67" s="126"/>
-      <c r="I67" s="128" t="s">
+      <c r="H67" s="124"/>
+      <c r="I67" s="126" t="s">
         <v>206</v>
       </c>
-      <c r="J67" s="128" t="s">
+      <c r="J67" s="126" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="121" t="s">
+      <c r="A68" s="119" t="s">
         <v>147</v>
       </c>
       <c r="B68" s="100">
@@ -11034,7 +13490,7 @@
       <c r="C68" s="97">
         <v>2</v>
       </c>
-      <c r="D68" s="114" t="s">
+      <c r="D68" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E68" s="97" t="s">
@@ -11045,16 +13501,16 @@
         <v>5</v>
       </c>
       <c r="G68" s="99"/>
-      <c r="H68" s="129" t="s">
+      <c r="H68" s="127" t="s">
         <v>208</v>
       </c>
-      <c r="I68" s="128" t="s">
+      <c r="I68" s="126" t="s">
         <v>209</v>
       </c>
-      <c r="J68" s="126"/>
+      <c r="J68" s="124"/>
     </row>
     <row r="69" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="122" t="s">
+      <c r="A69" s="120" t="s">
         <v>148</v>
       </c>
       <c r="B69" s="104">
@@ -11063,7 +13519,7 @@
       <c r="C69" s="105">
         <v>0</v>
       </c>
-      <c r="D69" s="114" t="s">
+      <c r="D69" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E69" s="105" t="s">
@@ -11074,32 +13530,32 @@
         <v>0</v>
       </c>
       <c r="G69" s="99"/>
-      <c r="H69" s="132" t="s">
+      <c r="H69" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="I69" s="132" t="s">
+      <c r="I69" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J69" s="126"/>
+      <c r="J69" s="124"/>
     </row>
     <row r="70" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="119" t="s">
+      <c r="A70" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B70" s="112">
+      <c r="B70" s="132">
         <v>58</v>
       </c>
-      <c r="C70" s="112"/>
-      <c r="D70" s="112"/>
-      <c r="E70" s="112"/>
-      <c r="F70" s="113"/>
+      <c r="C70" s="132"/>
+      <c r="D70" s="132"/>
+      <c r="E70" s="132"/>
+      <c r="F70" s="133"/>
       <c r="G70" s="102"/>
-      <c r="H70" s="130"/>
-      <c r="I70" s="130"/>
-      <c r="J70" s="130"/>
+      <c r="H70" s="128"/>
+      <c r="I70" s="128"/>
+      <c r="J70" s="128"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A71" s="133" t="s">
+      <c r="A71" s="131" t="s">
         <v>221</v>
       </c>
       <c r="G71" s="102"/>
@@ -11108,10 +13564,10 @@
       <c r="G72" s="102"/>
     </row>
     <row r="73" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="119" t="s">
+      <c r="A73" s="117" t="s">
         <v>157</v>
       </c>
-      <c r="B73" s="115" t="s">
+      <c r="B73" s="113" t="s">
         <v>135</v>
       </c>
       <c r="C73" s="108" t="s">
@@ -11127,21 +13583,21 @@
         <v>139</v>
       </c>
       <c r="G73" s="110"/>
-      <c r="H73" s="123" t="s">
+      <c r="H73" s="121" t="s">
         <v>140</v>
       </c>
-      <c r="I73" s="124" t="s">
+      <c r="I73" s="122" t="s">
         <v>141</v>
       </c>
-      <c r="J73" s="125" t="s">
+      <c r="J73" s="123" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A74" s="120" t="s">
+      <c r="A74" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B74" s="118" t="s">
+      <c r="B74" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C74" s="106">
@@ -11158,19 +13614,19 @@
         <v>2</v>
       </c>
       <c r="G74" s="99"/>
-      <c r="H74" s="126"/>
-      <c r="I74" s="127" t="s">
+      <c r="H74" s="124"/>
+      <c r="I74" s="125" t="s">
         <v>210</v>
       </c>
-      <c r="J74" s="127" t="s">
+      <c r="J74" s="125" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A75" s="121" t="s">
+      <c r="A75" s="119" t="s">
         <v>145</v>
       </c>
-      <c r="B75" s="118" t="s">
+      <c r="B75" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C75" s="97">
@@ -11187,19 +13643,19 @@
         <v>3</v>
       </c>
       <c r="G75" s="99"/>
-      <c r="H75" s="126"/>
-      <c r="I75" s="128" t="s">
+      <c r="H75" s="124"/>
+      <c r="I75" s="126" t="s">
         <v>211</v>
       </c>
-      <c r="J75" s="128" t="s">
+      <c r="J75" s="126" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A76" s="121" t="s">
+      <c r="A76" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="B76" s="118" t="s">
+      <c r="B76" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C76" s="97">
@@ -11216,16 +13672,16 @@
         <v>2</v>
       </c>
       <c r="G76" s="99"/>
-      <c r="H76" s="126"/>
-      <c r="I76" s="128" t="s">
+      <c r="H76" s="124"/>
+      <c r="I76" s="126" t="s">
         <v>206</v>
       </c>
-      <c r="J76" s="128" t="s">
+      <c r="J76" s="126" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="121" t="s">
+      <c r="A77" s="119" t="s">
         <v>147</v>
       </c>
       <c r="B77" s="100">
@@ -11234,7 +13690,7 @@
       <c r="C77" s="97">
         <v>3</v>
       </c>
-      <c r="D77" s="114" t="s">
+      <c r="D77" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E77" s="97" t="s">
@@ -11245,16 +13701,16 @@
         <v>6</v>
       </c>
       <c r="G77" s="99"/>
-      <c r="H77" s="129" t="s">
+      <c r="H77" s="127" t="s">
         <v>213</v>
       </c>
-      <c r="I77" s="128" t="s">
+      <c r="I77" s="126" t="s">
         <v>212</v>
       </c>
-      <c r="J77" s="126"/>
+      <c r="J77" s="124"/>
     </row>
     <row r="78" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="122" t="s">
+      <c r="A78" s="120" t="s">
         <v>148</v>
       </c>
       <c r="B78" s="104">
@@ -11263,7 +13719,7 @@
       <c r="C78" s="105">
         <v>0</v>
       </c>
-      <c r="D78" s="114" t="s">
+      <c r="D78" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E78" s="105" t="s">
@@ -11274,32 +13730,32 @@
         <v>0</v>
       </c>
       <c r="G78" s="99"/>
-      <c r="H78" s="132" t="s">
+      <c r="H78" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="I78" s="132" t="s">
+      <c r="I78" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J78" s="126"/>
+      <c r="J78" s="124"/>
     </row>
     <row r="79" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="119" t="s">
+      <c r="A79" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B79" s="112">
+      <c r="B79" s="132">
         <v>66</v>
       </c>
-      <c r="C79" s="112"/>
-      <c r="D79" s="112"/>
-      <c r="E79" s="112"/>
-      <c r="F79" s="113"/>
+      <c r="C79" s="132"/>
+      <c r="D79" s="132"/>
+      <c r="E79" s="132"/>
+      <c r="F79" s="133"/>
       <c r="G79" s="102"/>
-      <c r="H79" s="130"/>
-      <c r="I79" s="130"/>
-      <c r="J79" s="130"/>
+      <c r="H79" s="128"/>
+      <c r="I79" s="128"/>
+      <c r="J79" s="128"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A80" s="133" t="s">
+      <c r="A80" s="131" t="s">
         <v>222</v>
       </c>
       <c r="G80" s="102"/>
@@ -11308,10 +13764,10 @@
       <c r="G81" s="102"/>
     </row>
     <row r="82" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="119" t="s">
+      <c r="A82" s="117" t="s">
         <v>158</v>
       </c>
-      <c r="B82" s="115" t="s">
+      <c r="B82" s="113" t="s">
         <v>135</v>
       </c>
       <c r="C82" s="108" t="s">
@@ -11327,21 +13783,21 @@
         <v>139</v>
       </c>
       <c r="G82" s="110"/>
-      <c r="H82" s="123" t="s">
+      <c r="H82" s="121" t="s">
         <v>140</v>
       </c>
-      <c r="I82" s="124" t="s">
+      <c r="I82" s="122" t="s">
         <v>141</v>
       </c>
-      <c r="J82" s="125" t="s">
+      <c r="J82" s="123" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="120" t="s">
+      <c r="A83" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="B83" s="118" t="s">
+      <c r="B83" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C83" s="106">
@@ -11358,19 +13814,19 @@
         <v>4</v>
       </c>
       <c r="G83" s="99"/>
-      <c r="H83" s="126"/>
-      <c r="I83" s="127" t="s">
+      <c r="H83" s="124"/>
+      <c r="I83" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="J83" s="127" t="s">
+      <c r="J83" s="125" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A84" s="121" t="s">
+      <c r="A84" s="119" t="s">
         <v>145</v>
       </c>
-      <c r="B84" s="118" t="s">
+      <c r="B84" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C84" s="97">
@@ -11387,19 +13843,19 @@
         <v>4</v>
       </c>
       <c r="G84" s="99"/>
-      <c r="H84" s="126"/>
-      <c r="I84" s="128" t="s">
+      <c r="H84" s="124"/>
+      <c r="I84" s="126" t="s">
         <v>215</v>
       </c>
-      <c r="J84" s="128" t="s">
+      <c r="J84" s="126" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A85" s="121" t="s">
+      <c r="A85" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="B85" s="118" t="s">
+      <c r="B85" s="116" t="s">
         <v>128</v>
       </c>
       <c r="C85" s="97">
@@ -11416,16 +13872,16 @@
         <v>2</v>
       </c>
       <c r="G85" s="99"/>
-      <c r="H85" s="126"/>
-      <c r="I85" s="128" t="s">
+      <c r="H85" s="124"/>
+      <c r="I85" s="126" t="s">
         <v>216</v>
       </c>
-      <c r="J85" s="128" t="s">
+      <c r="J85" s="126" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A86" s="121" t="s">
+      <c r="A86" s="119" t="s">
         <v>147</v>
       </c>
       <c r="B86" s="100">
@@ -11434,7 +13890,7 @@
       <c r="C86" s="97">
         <v>3</v>
       </c>
-      <c r="D86" s="114" t="s">
+      <c r="D86" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E86" s="97" t="s">
@@ -11445,16 +13901,16 @@
         <v>6</v>
       </c>
       <c r="G86" s="99"/>
-      <c r="H86" s="129" t="s">
+      <c r="H86" s="127" t="s">
         <v>217</v>
       </c>
-      <c r="I86" s="128" t="s">
+      <c r="I86" s="126" t="s">
         <v>218</v>
       </c>
-      <c r="J86" s="126"/>
+      <c r="J86" s="124"/>
     </row>
     <row r="87" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="122" t="s">
+      <c r="A87" s="120" t="s">
         <v>148</v>
       </c>
       <c r="B87" s="104">
@@ -11463,7 +13919,7 @@
       <c r="C87" s="105">
         <v>0</v>
       </c>
-      <c r="D87" s="114" t="s">
+      <c r="D87" s="112" t="s">
         <v>128</v>
       </c>
       <c r="E87" s="105" t="s">
@@ -11474,32 +13930,32 @@
         <v>0</v>
       </c>
       <c r="G87" s="99"/>
-      <c r="H87" s="132" t="s">
+      <c r="H87" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="I87" s="132" t="s">
+      <c r="I87" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="J87" s="126"/>
+      <c r="J87" s="124"/>
     </row>
     <row r="88" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="119" t="s">
+      <c r="A88" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B88" s="112">
+      <c r="B88" s="132">
         <v>76</v>
       </c>
-      <c r="C88" s="112"/>
-      <c r="D88" s="112"/>
-      <c r="E88" s="112"/>
-      <c r="F88" s="113"/>
+      <c r="C88" s="132"/>
+      <c r="D88" s="132"/>
+      <c r="E88" s="132"/>
+      <c r="F88" s="133"/>
       <c r="G88" s="102"/>
-      <c r="H88" s="130"/>
-      <c r="I88" s="130"/>
-      <c r="J88" s="130"/>
+      <c r="H88" s="128"/>
+      <c r="I88" s="128"/>
+      <c r="J88" s="128"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A89" s="133" t="s">
+      <c r="A89" s="131" t="s">
         <v>223</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update TimeSheet (Week 17/18)
</commit_message>
<xml_diff>
--- a/midterm-presentation/TimeSheet.xlsx
+++ b/midterm-presentation/TimeSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programmierung\Android\Tower-Defense\midterm-presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B10EBF-C9AB-411A-9DA3-98FE0FE7CD38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93E1A88-250B-460C-94AA-CB76BBFE4A05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="368">
   <si>
     <t>Ticketart</t>
   </si>
@@ -1028,6 +1028,117 @@
   </si>
   <si>
     <t>Project Management (h)</t>
+  </si>
+  <si>
+    <t>DHTD-104</t>
+  </si>
+  <si>
+    <t>Create design for car enemy</t>
+  </si>
+  <si>
+    <t>DHTD-107</t>
+  </si>
+  <si>
+    <t>Transition</t>
+  </si>
+  <si>
+    <t>Update Time Sheet (Sprint 11-16)</t>
+  </si>
+  <si>
+    <t>DHTD-108</t>
+  </si>
+  <si>
+    <t>Blog Entry Week 17</t>
+  </si>
+  <si>
+    <t>DHTD-109</t>
+  </si>
+  <si>
+    <t>Write comments to other groups (Week 17)</t>
+  </si>
+  <si>
+    <t>DHTD-110</t>
+  </si>
+  <si>
+    <t>Create levels for towers</t>
+  </si>
+  <si>
+    <t>DHTD-111</t>
+  </si>
+  <si>
+    <t>Lasertower: Check if it is posssible to make multiple damage</t>
+  </si>
+  <si>
+    <t>DHTD-112</t>
+  </si>
+  <si>
+    <t>Refactor code snippets according to Metrics</t>
+  </si>
+  <si>
+    <t>DHTD-113</t>
+  </si>
+  <si>
+    <t>Improve Test Automation</t>
+  </si>
+  <si>
+    <t>DHTD-84</t>
+  </si>
+  <si>
+    <t>Implement new enemy car</t>
+  </si>
+  <si>
+    <t>DHTD-85</t>
+  </si>
+  <si>
+    <t>implement new enemy plane</t>
+  </si>
+  <si>
+    <t>DHTD-88</t>
+  </si>
+  <si>
+    <t>Design the easy match</t>
+  </si>
+  <si>
+    <t>DHTD-91</t>
+  </si>
+  <si>
+    <t>Implement boss enemy</t>
+  </si>
+  <si>
+    <t>DHTD-106</t>
+  </si>
+  <si>
+    <t>Bug: Tower Radius is below newly spawned enemies</t>
+  </si>
+  <si>
+    <t>DHTD-114</t>
+  </si>
+  <si>
+    <t>Ingame Music</t>
+  </si>
+  <si>
+    <t>DHTD-115</t>
+  </si>
+  <si>
+    <t>Bugfixes</t>
+  </si>
+  <si>
+    <t>DHTD-116</t>
+  </si>
+  <si>
+    <t>Blog Entry Week 18</t>
+  </si>
+  <si>
+    <t>DHTD-117</t>
+  </si>
+  <si>
+    <t>Create question formular for UX test</t>
+  </si>
+  <si>
+    <t>DHTD-118</t>
+  </si>
+  <si>
+    <t>Create design for plane enemy</t>
   </si>
 </sst>
 </file>
@@ -1928,12 +2039,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1942,6 +2047,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -9610,9 +9721,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50C860A-1B08-4855-95EB-100DD969983E}">
-  <dimension ref="A1:Q93"/>
+  <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -9675,31 +9788,31 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="132" t="s">
         <v>224</v>
       </c>
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="133" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="135" t="s">
+      <c r="C2" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="136" t="s">
+      <c r="D2" s="134" t="s">
         <v>225</v>
       </c>
-      <c r="E2" s="135" t="s">
+      <c r="E2" s="133" t="s">
         <v>226</v>
       </c>
-      <c r="F2" s="135">
+      <c r="F2" s="133">
         <v>2</v>
       </c>
-      <c r="G2" s="135">
+      <c r="G2" s="133">
         <v>3.75</v>
       </c>
-      <c r="H2" s="135" t="s">
+      <c r="H2" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="137">
+      <c r="I2" s="135">
         <v>0.5</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -9715,17 +9828,17 @@
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" s="138"/>
-      <c r="B3" s="138"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138" t="s">
+      <c r="A3" s="136"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="138">
+      <c r="I3" s="136">
         <v>2.5</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -10091,8 +10204,8 @@
         <v>226</v>
       </c>
       <c r="M17" s="5">
-        <f>SUM(G2,G55/2)</f>
-        <v>11.125</v>
+        <f>SUM(G2,G55/2,G100)</f>
+        <v>12.375</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
@@ -11689,6 +11802,629 @@
         <v>22</v>
       </c>
       <c r="I93" s="1">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>331</v>
+      </c>
+      <c r="B94" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" t="s">
+        <v>57</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F94">
+        <v>3</v>
+      </c>
+      <c r="G94">
+        <v>3.5</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I94" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>333</v>
+      </c>
+      <c r="B95" t="s">
+        <v>242</v>
+      </c>
+      <c r="C95" t="s">
+        <v>334</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
+      </c>
+      <c r="G95">
+        <v>1.25</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I95" s="1">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>336</v>
+      </c>
+      <c r="B96" t="s">
+        <v>242</v>
+      </c>
+      <c r="C96" t="s">
+        <v>57</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="F96">
+        <v>2.5</v>
+      </c>
+      <c r="G96">
+        <v>3</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I96" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H97" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I97" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H98" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I98" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>338</v>
+      </c>
+      <c r="B99" t="s">
+        <v>242</v>
+      </c>
+      <c r="C99" t="s">
+        <v>57</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I99" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>340</v>
+      </c>
+      <c r="B100" t="s">
+        <v>52</v>
+      </c>
+      <c r="C100" t="s">
+        <v>57</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E100" t="s">
+        <v>226</v>
+      </c>
+      <c r="F100">
+        <v>2</v>
+      </c>
+      <c r="G100">
+        <v>1.25</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I100" s="1">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>342</v>
+      </c>
+      <c r="B101" t="s">
+        <v>52</v>
+      </c>
+      <c r="C101" t="s">
+        <v>57</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="F101">
+        <v>3</v>
+      </c>
+      <c r="G101">
+        <v>1.5</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I101" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H102" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I102" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H103" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I103" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>344</v>
+      </c>
+      <c r="B104" t="s">
+        <v>43</v>
+      </c>
+      <c r="C104" t="s">
+        <v>57</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F104">
+        <v>6</v>
+      </c>
+      <c r="G104">
+        <v>5.25</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I104" s="1">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>346</v>
+      </c>
+      <c r="B105" t="s">
+        <v>43</v>
+      </c>
+      <c r="C105" t="s">
+        <v>57</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F105">
+        <v>8</v>
+      </c>
+      <c r="G105">
+        <v>6.25</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I105" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H106" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I106" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H107" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I107" s="1">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>348</v>
+      </c>
+      <c r="B108" t="s">
+        <v>52</v>
+      </c>
+      <c r="C108" t="s">
+        <v>57</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="F108">
+        <v>4</v>
+      </c>
+      <c r="G108">
+        <v>2</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I108" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H109" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I109" s="1">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>350</v>
+      </c>
+      <c r="B110" t="s">
+        <v>52</v>
+      </c>
+      <c r="C110" t="s">
+        <v>57</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="F110">
+        <v>3</v>
+      </c>
+      <c r="G110">
+        <v>2.75</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I110" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H111" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I111" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H112" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I112" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>352</v>
+      </c>
+      <c r="B113" t="s">
+        <v>52</v>
+      </c>
+      <c r="C113" t="s">
+        <v>57</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F113">
+        <v>4</v>
+      </c>
+      <c r="G113">
+        <v>2.75</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I113" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H114" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I114" s="1">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H115" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I115" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>354</v>
+      </c>
+      <c r="B116" t="s">
+        <v>52</v>
+      </c>
+      <c r="C116" t="s">
+        <v>57</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="F116">
+        <v>4</v>
+      </c>
+      <c r="G116">
+        <v>3.75</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I116" s="1">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H117" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I117" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H118" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I118" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>356</v>
+      </c>
+      <c r="B119" t="s">
+        <v>52</v>
+      </c>
+      <c r="C119" t="s">
+        <v>57</v>
+      </c>
+      <c r="D119" t="s">
+        <v>357</v>
+      </c>
+      <c r="F119">
+        <v>3</v>
+      </c>
+      <c r="G119">
+        <v>0.25</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I119" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>358</v>
+      </c>
+      <c r="B120" t="s">
+        <v>52</v>
+      </c>
+      <c r="C120" t="s">
+        <v>57</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="F120">
+        <v>14</v>
+      </c>
+      <c r="G120">
+        <v>14</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I120" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>360</v>
+      </c>
+      <c r="B121" t="s">
+        <v>52</v>
+      </c>
+      <c r="C121" t="s">
+        <v>334</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="F121">
+        <v>4</v>
+      </c>
+      <c r="G121">
+        <v>3</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I121" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H122" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I122" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H123" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I123" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>362</v>
+      </c>
+      <c r="B124" t="s">
+        <v>242</v>
+      </c>
+      <c r="C124" t="s">
+        <v>57</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="F124">
+        <v>1</v>
+      </c>
+      <c r="G124">
+        <v>1.5</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I124" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H125" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I125" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H126" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I126" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>364</v>
+      </c>
+      <c r="B127" t="s">
+        <v>43</v>
+      </c>
+      <c r="C127" t="s">
+        <v>334</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="F127">
+        <v>3</v>
+      </c>
+      <c r="G127">
+        <v>2.25</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I127" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H128" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I128" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H129" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I129" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>366</v>
+      </c>
+      <c r="B130" t="s">
+        <v>18</v>
+      </c>
+      <c r="C130" t="s">
+        <v>19</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F130">
+        <v>3</v>
+      </c>
+      <c r="G130">
+        <v>2.75</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I130" s="1">
         <v>2.75</v>
       </c>
     </row>
@@ -12168,13 +12904,13 @@
       <c r="A7" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="132">
+      <c r="B7" s="137">
         <v>82</v>
       </c>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132"/>
-      <c r="E7" s="132"/>
-      <c r="F7" s="133"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="138"/>
       <c r="G7" s="102"/>
       <c r="H7" s="128"/>
       <c r="I7" s="128"/>
@@ -12360,13 +13096,13 @@
       <c r="A16" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B16" s="132">
+      <c r="B16" s="137">
         <v>81</v>
       </c>
-      <c r="C16" s="132"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="133"/>
+      <c r="C16" s="137"/>
+      <c r="D16" s="137"/>
+      <c r="E16" s="137"/>
+      <c r="F16" s="138"/>
       <c r="G16" s="102"/>
       <c r="H16" s="128"/>
       <c r="I16" s="128"/>
@@ -12552,13 +13288,13 @@
       <c r="A25" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B25" s="132">
+      <c r="B25" s="137">
         <v>64</v>
       </c>
-      <c r="C25" s="132"/>
-      <c r="D25" s="132"/>
-      <c r="E25" s="132"/>
-      <c r="F25" s="133"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="137"/>
+      <c r="E25" s="137"/>
+      <c r="F25" s="138"/>
       <c r="G25" s="102"/>
       <c r="H25" s="128"/>
       <c r="I25" s="128"/>
@@ -12744,13 +13480,13 @@
       <c r="A34" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B34" s="132">
+      <c r="B34" s="137">
         <v>44</v>
       </c>
-      <c r="C34" s="132"/>
-      <c r="D34" s="132"/>
-      <c r="E34" s="132"/>
-      <c r="F34" s="133"/>
+      <c r="C34" s="137"/>
+      <c r="D34" s="137"/>
+      <c r="E34" s="137"/>
+      <c r="F34" s="138"/>
       <c r="G34" s="102"/>
       <c r="H34" s="128"/>
       <c r="I34" s="128"/>
@@ -12942,13 +13678,13 @@
       <c r="A43" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B43" s="132">
+      <c r="B43" s="137">
         <v>80</v>
       </c>
-      <c r="C43" s="132"/>
-      <c r="D43" s="132"/>
-      <c r="E43" s="132"/>
-      <c r="F43" s="133"/>
+      <c r="C43" s="137"/>
+      <c r="D43" s="137"/>
+      <c r="E43" s="137"/>
+      <c r="F43" s="138"/>
       <c r="G43" s="102"/>
       <c r="H43" s="128"/>
       <c r="I43" s="128"/>
@@ -13142,13 +13878,13 @@
       <c r="A52" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B52" s="132">
+      <c r="B52" s="137">
         <v>80</v>
       </c>
-      <c r="C52" s="132"/>
-      <c r="D52" s="132"/>
-      <c r="E52" s="132"/>
-      <c r="F52" s="133"/>
+      <c r="C52" s="137"/>
+      <c r="D52" s="137"/>
+      <c r="E52" s="137"/>
+      <c r="F52" s="138"/>
       <c r="G52" s="102"/>
       <c r="H52" s="128"/>
       <c r="I52" s="128"/>
@@ -13342,13 +14078,13 @@
       <c r="A61" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B61" s="132">
+      <c r="B61" s="137">
         <v>79</v>
       </c>
-      <c r="C61" s="132"/>
-      <c r="D61" s="132"/>
-      <c r="E61" s="132"/>
-      <c r="F61" s="133"/>
+      <c r="C61" s="137"/>
+      <c r="D61" s="137"/>
+      <c r="E61" s="137"/>
+      <c r="F61" s="138"/>
       <c r="G61" s="102"/>
       <c r="H61" s="128"/>
       <c r="I61" s="128"/>
@@ -13542,13 +14278,13 @@
       <c r="A70" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B70" s="132">
+      <c r="B70" s="137">
         <v>58</v>
       </c>
-      <c r="C70" s="132"/>
-      <c r="D70" s="132"/>
-      <c r="E70" s="132"/>
-      <c r="F70" s="133"/>
+      <c r="C70" s="137"/>
+      <c r="D70" s="137"/>
+      <c r="E70" s="137"/>
+      <c r="F70" s="138"/>
       <c r="G70" s="102"/>
       <c r="H70" s="128"/>
       <c r="I70" s="128"/>
@@ -13742,13 +14478,13 @@
       <c r="A79" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B79" s="132">
+      <c r="B79" s="137">
         <v>66</v>
       </c>
-      <c r="C79" s="132"/>
-      <c r="D79" s="132"/>
-      <c r="E79" s="132"/>
-      <c r="F79" s="133"/>
+      <c r="C79" s="137"/>
+      <c r="D79" s="137"/>
+      <c r="E79" s="137"/>
+      <c r="F79" s="138"/>
       <c r="G79" s="102"/>
       <c r="H79" s="128"/>
       <c r="I79" s="128"/>
@@ -13942,13 +14678,13 @@
       <c r="A88" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B88" s="132">
+      <c r="B88" s="137">
         <v>76</v>
       </c>
-      <c r="C88" s="132"/>
-      <c r="D88" s="132"/>
-      <c r="E88" s="132"/>
-      <c r="F88" s="133"/>
+      <c r="C88" s="137"/>
+      <c r="D88" s="137"/>
+      <c r="E88" s="137"/>
+      <c r="F88" s="138"/>
       <c r="G88" s="102"/>
       <c r="H88" s="128"/>
       <c r="I88" s="128"/>

</xml_diff>

<commit_message>
Update Time Sheet (Week 19)
</commit_message>
<xml_diff>
--- a/midterm-presentation/TimeSheet.xlsx
+++ b/midterm-presentation/TimeSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programmierung\Android\Tower-Defense\midterm-presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93E1A88-250B-460C-94AA-CB76BBFE4A05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56896447-1227-4DAB-B9BE-D5F22FB7FE18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="379">
   <si>
     <t>Ticketart</t>
   </si>
@@ -1139,6 +1139,39 @@
   </si>
   <si>
     <t>Create design for plane enemy</t>
+  </si>
+  <si>
+    <t>DHTD-89</t>
+  </si>
+  <si>
+    <t>Design the medium match</t>
+  </si>
+  <si>
+    <t>DHTD-90</t>
+  </si>
+  <si>
+    <t>Design the hard match</t>
+  </si>
+  <si>
+    <t>DHTD-119</t>
+  </si>
+  <si>
+    <t>Implement enemy life bar</t>
+  </si>
+  <si>
+    <t>DHTD-120</t>
+  </si>
+  <si>
+    <t>DHTD-121</t>
+  </si>
+  <si>
+    <t>Balancing</t>
+  </si>
+  <si>
+    <t>DHTD-122</t>
+  </si>
+  <si>
+    <t>Blog Entry Week 19</t>
   </si>
 </sst>
 </file>
@@ -9721,10 +9754,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50C860A-1B08-4855-95EB-100DD969983E}">
-  <dimension ref="A1:Q130"/>
+  <dimension ref="A1:Q139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12426,6 +12459,186 @@
       </c>
       <c r="I130" s="1">
         <v>2.75</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>368</v>
+      </c>
+      <c r="B131" t="s">
+        <v>52</v>
+      </c>
+      <c r="C131" t="s">
+        <v>57</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="F131">
+        <v>2</v>
+      </c>
+      <c r="G131">
+        <v>1.5</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I131" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>370</v>
+      </c>
+      <c r="B132" t="s">
+        <v>52</v>
+      </c>
+      <c r="C132" t="s">
+        <v>57</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="F132">
+        <v>3</v>
+      </c>
+      <c r="G132">
+        <v>1</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I132" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>372</v>
+      </c>
+      <c r="B133" t="s">
+        <v>52</v>
+      </c>
+      <c r="C133" t="s">
+        <v>57</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="F133">
+        <v>4</v>
+      </c>
+      <c r="G133">
+        <v>4</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I133" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>374</v>
+      </c>
+      <c r="B134" t="s">
+        <v>52</v>
+      </c>
+      <c r="C134" t="s">
+        <v>57</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="F134">
+        <v>6</v>
+      </c>
+      <c r="G134">
+        <v>10.75</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I134" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H135" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I135" s="1">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>375</v>
+      </c>
+      <c r="B136" t="s">
+        <v>18</v>
+      </c>
+      <c r="C136" t="s">
+        <v>334</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="F136">
+        <v>4</v>
+      </c>
+      <c r="G136">
+        <v>0.5</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I136" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>377</v>
+      </c>
+      <c r="B137" t="s">
+        <v>242</v>
+      </c>
+      <c r="C137" t="s">
+        <v>334</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="F137">
+        <v>2.5</v>
+      </c>
+      <c r="G137">
+        <v>1.75</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I137" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H138" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I138" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H139" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I139" s="1">
+        <v>1.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Time Sheet (Week 20)
</commit_message>
<xml_diff>
--- a/midterm-presentation/TimeSheet.xlsx
+++ b/midterm-presentation/TimeSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programmierung\Android\Tower-Defense\midterm-presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56896447-1227-4DAB-B9BE-D5F22FB7FE18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16594F2F-0F45-4FB1-9444-D017476C3003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="383">
   <si>
     <t>Ticketart</t>
   </si>
@@ -1172,6 +1172,18 @@
   </si>
   <si>
     <t>Blog Entry Week 19</t>
+  </si>
+  <si>
+    <t>DHTD-124</t>
+  </si>
+  <si>
+    <t>Blog Entry Week 20</t>
+  </si>
+  <si>
+    <t>DHTD-125</t>
+  </si>
+  <si>
+    <t>Carry out Usability Test</t>
   </si>
 </sst>
 </file>
@@ -9754,10 +9766,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50C860A-1B08-4855-95EB-100DD969983E}">
-  <dimension ref="A1:Q139"/>
+  <dimension ref="A1:Q145"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140"/>
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12639,6 +12651,90 @@
       </c>
       <c r="I139" s="1">
         <v>1.25</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>379</v>
+      </c>
+      <c r="B140" t="s">
+        <v>242</v>
+      </c>
+      <c r="C140" t="s">
+        <v>334</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="F140">
+        <v>1.5</v>
+      </c>
+      <c r="G140">
+        <v>2</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I140" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H141" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I141" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H142" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I142" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>381</v>
+      </c>
+      <c r="B143" t="s">
+        <v>43</v>
+      </c>
+      <c r="C143" t="s">
+        <v>334</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="F143">
+        <v>2</v>
+      </c>
+      <c r="G143">
+        <v>1.5</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I143" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H144" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I144" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="145" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H145" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I145" s="1">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Function Points Diagrams
</commit_message>
<xml_diff>
--- a/midterm-presentation/TimeSheet.xlsx
+++ b/midterm-presentation/TimeSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programmierung\Android\Tower-Defense\midterm-presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE2BE78-C1C2-4B78-83F0-4F26E4D04C33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E29A24-1BED-4A5C-8E15-32AB57B715D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TicketLog3rdS" sheetId="1" r:id="rId1"/>
@@ -2100,13 +2100,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Akzent3" xfId="1" builtinId="37"/>
@@ -2910,8 +2910,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-9.3042448502845709E-2"/>
-                  <c:y val="-6.8529627212587402E-2"/>
+                  <c:x val="2.1032972351965971E-2"/>
+                  <c:y val="-1.3664668721762601E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2919,7 +2919,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CDDA7B28-6582-4E89-BB49-F15A92DD12C5}" type="CELLRANGE">
+                    <a:fld id="{22D4B61D-92D5-46E8-81B1-9DEB176495CA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2949,8 +2949,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.11124523343697812"/>
-                  <c:y val="-5.6553837995549784E-2"/>
+                  <c:x val="-9.015090321605862E-2"/>
+                  <c:y val="-4.9695718184196679E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2958,163 +2958,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{927BE7D3-B806-4CFE-8605-55BD1CFE505C}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="de-DE"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="1"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000E-F948-4DA7-9538-26EF1BE05274}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-8.7556639032845482E-2"/>
-                  <c:y val="6.8632769014474626E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{3A435C1C-00F7-4753-9C3D-97A220A083A4}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="de-DE"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="1"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000F-F948-4DA7-9538-26EF1BE05274}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.8386854084005014E-2"/>
-                  <c:y val="6.8632769014474682E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{6601609D-EF55-43D8-9E51-D5335665D880}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="de-DE"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="1"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000010-F948-4DA7-9538-26EF1BE05274}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="4.0518478449645618E-3"/>
-                  <c:y val="-6.8065489104094648E-3"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{22D4B61D-92D5-46E8-81B1-9DEB176495CA}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="de-DE"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="1"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000011-F948-4DA7-9538-26EF1BE05274}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-9.015090321605862E-2"/>
-                  <c:y val="3.945983936339368E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{07234101-ADBB-43C2-B451-7602E2EE1370}" type="CELLRANGE">
+                    <a:fld id="{1197BB59-F954-490E-8E3E-AFE2AA9CB4EC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -3136,12 +2980,12 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000012-F948-4DA7-9538-26EF1BE05274}"/>
+                  <c16:uniqueId val="{0000000E-F948-4DA7-9538-26EF1BE05274}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="6"/>
+              <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-5.1538084294420909E-2"/>
@@ -3175,12 +3019,12 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000013-F948-4DA7-9538-26EF1BE05274}"/>
+                  <c16:uniqueId val="{0000000F-F948-4DA7-9538-26EF1BE05274}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="7"/>
+              <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-4.8594392247336693E-2"/>
@@ -3214,12 +3058,12 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000014-F948-4DA7-9538-26EF1BE05274}"/>
+                  <c16:uniqueId val="{00000010-F948-4DA7-9538-26EF1BE05274}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="8"/>
+              <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-5.6278388228321999E-2"/>
@@ -3253,12 +3097,12 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000015-F948-4DA7-9538-26EF1BE05274}"/>
+                  <c16:uniqueId val="{00000011-F948-4DA7-9538-26EF1BE05274}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="9"/>
+              <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-2.5901043276908359E-2"/>
@@ -3292,7 +3136,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000016-F948-4DA7-9538-26EF1BE05274}"/>
+                  <c16:uniqueId val="{00000012-F948-4DA7-9538-26EF1BE05274}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3354,76 +3198,340 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Use Case Overview'!$G$7:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>12.375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Use Case Overview'!$H$7:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>'Use Case Overview'!$B$7:$B$12</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>Upgrade Towers</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Sell Towers</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Select between different Towers</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Edit Settings</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Toggle Sound &amp; Animations</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Choose Difficulties</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000019-F948-4DA7-9538-26EF1BE05274}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Time spent 1-4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5306616265064806E-2"/>
+                  <c:y val="-8.9103986646646718E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{CDDA7B28-6582-4E89-BB49-F15A92DD12C5}" type="CELLRANGE">
+                      <a:rPr lang="en-US" sz="900"/>
+                      <a:pPr/>
+                      <a:t>[ZELLBEREICH]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-DE"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-F392-4901-8439-7366A9F23BD8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.11124523343697812"/>
+                  <c:y val="5.6605138891776437E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{927BE7D3-B806-4CFE-8605-55BD1CFE505C}" type="CELLRANGE">
+                      <a:rPr lang="en-US" sz="900"/>
+                      <a:pPr/>
+                      <a:t>[ZELLBEREICH]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-DE"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-F392-4901-8439-7366A9F23BD8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.0009472585289301E-2"/>
+                  <c:y val="9.2636188354210544E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{3A435C1C-00F7-4753-9C3D-97A220A083A4}" type="CELLRANGE">
+                      <a:rPr lang="en-US" sz="900"/>
+                      <a:pPr/>
+                      <a:t>[ZELLBEREICH]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-DE"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-F392-4901-8439-7366A9F23BD8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.8386854084005014E-2"/>
+                  <c:y val="6.8632769014474682E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{6601609D-EF55-43D8-9E51-D5335665D880}" type="CELLRANGE">
+                      <a:rPr lang="en-US" sz="900"/>
+                      <a:pPr/>
+                      <a:t>[ZELLBEREICH]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-DE"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-F392-4901-8439-7366A9F23BD8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.4327865266841645E-2"/>
-                  <c:y val="-0.14422076272723974"/>
+                  <c:x val="0.49004375722310628"/>
+                  <c:y val="-0.20782506070381049"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="800" baseline="0"/>
+                      <a:t>y = 3,7778x + 41,778</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="800"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
-                </a:p>
-              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Use Case Overview'!$G$3:$G$12</c:f>
+              <c:f>'Use Case Overview'!$G$3:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>12</c:v>
                 </c:pt>
@@ -3436,33 +3544,15 @@
                 <c:pt idx="3">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>12.375</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10.125</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15.5</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Use Case Overview'!$H$3:$H$12</c:f>
+              <c:f>'Use Case Overview'!$H$3:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>82</c:v>
                 </c:pt>
@@ -3474,24 +3564,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3537,7 +3609,7 @@
               </c15:datalabelsRange>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000019-F948-4DA7-9538-26EF1BE05274}"/>
+              <c16:uniqueId val="{00000002-F392-4901-8439-7366A9F23BD8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3892,7 +3964,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ACB77D10-9791-45AC-80EE-91F46D1AFBA6}" type="CELLRANGE">
+                    <a:fld id="{6E25B8B2-9D7F-4D33-8563-AC9ECCB9DCB1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -5917,13 +5989,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>55.75</c:v>
+                  <c:v>55,75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44.75</c:v>
+                  <c:v>44,75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.91</c:v>
+                  <c:v>74,91</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -14443,7 +14515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50C860A-1B08-4855-95EB-100DD969983E}">
   <dimension ref="A1:Q145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+    <sheetView topLeftCell="A115" workbookViewId="0">
       <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
@@ -17688,7 +17760,7 @@
         <f>'FP Calculation'!$B$7</f>
         <v>82</v>
       </c>
-      <c r="I3" s="139" t="s">
+      <c r="I3" s="137" t="s">
         <v>127</v>
       </c>
     </row>
@@ -17722,7 +17794,7 @@
         <f>'FP Calculation'!B16</f>
         <v>81</v>
       </c>
-      <c r="I4" s="139" t="s">
+      <c r="I4" s="137" t="s">
         <v>127</v>
       </c>
     </row>
@@ -17757,7 +17829,7 @@
         <f>'FP Calculation'!B25</f>
         <v>64</v>
       </c>
-      <c r="I5" s="139" t="s">
+      <c r="I5" s="137" t="s">
         <v>127</v>
       </c>
     </row>
@@ -17792,7 +17864,7 @@
         <f>'FP Calculation'!B34</f>
         <v>44</v>
       </c>
-      <c r="I6" s="139" t="s">
+      <c r="I6" s="137" t="s">
         <v>127</v>
       </c>
     </row>
@@ -17995,7 +18067,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3800D6FA-69EA-4E12-9E16-1909B3CAE7B3}">
   <dimension ref="A1:Q89"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -18211,13 +18285,13 @@
       <c r="A7" s="117" t="s">
         <v>148</v>
       </c>
-      <c r="B7" s="137">
+      <c r="B7" s="138">
         <v>82</v>
       </c>
-      <c r="C7" s="137"/>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="139"/>
       <c r="G7" s="102"/>
       <c r="H7" s="128"/>
       <c r="I7" s="128"/>
@@ -18403,13 +18477,13 @@
       <c r="A16" s="117" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="137">
+      <c r="B16" s="138">
         <v>81</v>
       </c>
-      <c r="C16" s="137"/>
-      <c r="D16" s="137"/>
-      <c r="E16" s="137"/>
-      <c r="F16" s="138"/>
+      <c r="C16" s="138"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="138"/>
+      <c r="F16" s="139"/>
       <c r="G16" s="102"/>
       <c r="H16" s="128"/>
       <c r="I16" s="128"/>
@@ -18595,13 +18669,13 @@
       <c r="A25" s="117" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="137">
+      <c r="B25" s="138">
         <v>64</v>
       </c>
-      <c r="C25" s="137"/>
-      <c r="D25" s="137"/>
-      <c r="E25" s="137"/>
-      <c r="F25" s="138"/>
+      <c r="C25" s="138"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="138"/>
+      <c r="F25" s="139"/>
       <c r="G25" s="102"/>
       <c r="H25" s="128"/>
       <c r="I25" s="128"/>
@@ -18787,13 +18861,13 @@
       <c r="A34" s="117" t="s">
         <v>148</v>
       </c>
-      <c r="B34" s="137">
+      <c r="B34" s="138">
         <v>44</v>
       </c>
-      <c r="C34" s="137"/>
-      <c r="D34" s="137"/>
-      <c r="E34" s="137"/>
-      <c r="F34" s="138"/>
+      <c r="C34" s="138"/>
+      <c r="D34" s="138"/>
+      <c r="E34" s="138"/>
+      <c r="F34" s="139"/>
       <c r="G34" s="102"/>
       <c r="H34" s="128"/>
       <c r="I34" s="128"/>
@@ -18985,13 +19059,13 @@
       <c r="A43" s="117" t="s">
         <v>148</v>
       </c>
-      <c r="B43" s="137">
+      <c r="B43" s="138">
         <v>80</v>
       </c>
-      <c r="C43" s="137"/>
-      <c r="D43" s="137"/>
-      <c r="E43" s="137"/>
-      <c r="F43" s="138"/>
+      <c r="C43" s="138"/>
+      <c r="D43" s="138"/>
+      <c r="E43" s="138"/>
+      <c r="F43" s="139"/>
       <c r="G43" s="102"/>
       <c r="H43" s="128"/>
       <c r="I43" s="128"/>
@@ -19185,13 +19259,13 @@
       <c r="A52" s="117" t="s">
         <v>148</v>
       </c>
-      <c r="B52" s="137">
+      <c r="B52" s="138">
         <v>80</v>
       </c>
-      <c r="C52" s="137"/>
-      <c r="D52" s="137"/>
-      <c r="E52" s="137"/>
-      <c r="F52" s="138"/>
+      <c r="C52" s="138"/>
+      <c r="D52" s="138"/>
+      <c r="E52" s="138"/>
+      <c r="F52" s="139"/>
       <c r="G52" s="102"/>
       <c r="H52" s="128"/>
       <c r="I52" s="128"/>
@@ -19385,13 +19459,13 @@
       <c r="A61" s="117" t="s">
         <v>148</v>
       </c>
-      <c r="B61" s="137">
+      <c r="B61" s="138">
         <v>79</v>
       </c>
-      <c r="C61" s="137"/>
-      <c r="D61" s="137"/>
-      <c r="E61" s="137"/>
-      <c r="F61" s="138"/>
+      <c r="C61" s="138"/>
+      <c r="D61" s="138"/>
+      <c r="E61" s="138"/>
+      <c r="F61" s="139"/>
       <c r="G61" s="102"/>
       <c r="H61" s="128"/>
       <c r="I61" s="128"/>
@@ -19585,13 +19659,13 @@
       <c r="A70" s="117" t="s">
         <v>148</v>
       </c>
-      <c r="B70" s="137">
+      <c r="B70" s="138">
         <v>58</v>
       </c>
-      <c r="C70" s="137"/>
-      <c r="D70" s="137"/>
-      <c r="E70" s="137"/>
-      <c r="F70" s="138"/>
+      <c r="C70" s="138"/>
+      <c r="D70" s="138"/>
+      <c r="E70" s="138"/>
+      <c r="F70" s="139"/>
       <c r="G70" s="102"/>
       <c r="H70" s="128"/>
       <c r="I70" s="128"/>
@@ -19785,13 +19859,13 @@
       <c r="A79" s="117" t="s">
         <v>148</v>
       </c>
-      <c r="B79" s="137">
+      <c r="B79" s="138">
         <v>66</v>
       </c>
-      <c r="C79" s="137"/>
-      <c r="D79" s="137"/>
-      <c r="E79" s="137"/>
-      <c r="F79" s="138"/>
+      <c r="C79" s="138"/>
+      <c r="D79" s="138"/>
+      <c r="E79" s="138"/>
+      <c r="F79" s="139"/>
       <c r="G79" s="102"/>
       <c r="H79" s="128"/>
       <c r="I79" s="128"/>
@@ -19985,13 +20059,13 @@
       <c r="A88" s="117" t="s">
         <v>148</v>
       </c>
-      <c r="B88" s="137">
+      <c r="B88" s="138">
         <v>76</v>
       </c>
-      <c r="C88" s="137"/>
-      <c r="D88" s="137"/>
-      <c r="E88" s="137"/>
-      <c r="F88" s="138"/>
+      <c r="C88" s="138"/>
+      <c r="D88" s="138"/>
+      <c r="E88" s="138"/>
+      <c r="F88" s="139"/>
       <c r="G88" s="102"/>
       <c r="H88" s="128"/>
       <c r="I88" s="128"/>

</xml_diff>